<commit_message>
Disposition Reporting mapping update.  removed "flat file" column.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="478">
   <si>
     <t>Submitted Date</t>
   </si>
@@ -1227,84 +1227,6 @@
   </si>
   <si>
     <t>Sentence Term: Incarceration</t>
-  </si>
-  <si>
-    <t>Flat File ?</t>
-  </si>
-  <si>
-    <t>CASEID</t>
-  </si>
-  <si>
-    <t>PARTY-ID</t>
-  </si>
-  <si>
-    <t>COUNT-RECORD</t>
-  </si>
-  <si>
-    <t>CNT-CHG-NO</t>
-  </si>
-  <si>
-    <t>CNT-ARR-NO</t>
-  </si>
-  <si>
-    <t>SID-NO</t>
-  </si>
-  <si>
-    <t>DEF-NAME</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>SSN</t>
-  </si>
-  <si>
-    <t>CNT-INIT-CHG</t>
-  </si>
-  <si>
-    <t>CNT-INIT-SEVERITY</t>
-  </si>
-  <si>
-    <t>CNT-FIN-CHG</t>
-  </si>
-  <si>
-    <t>CNT-FIN-SEVERITY</t>
-  </si>
-  <si>
-    <t>CNT-DISP</t>
-  </si>
-  <si>
-    <t>CNT-FIN-PLEA</t>
-  </si>
-  <si>
-    <t>COUNSEL-TYPE</t>
-  </si>
-  <si>
-    <t>APP-TRL-TYPE</t>
-  </si>
-  <si>
-    <t>APP-JUDGE-ID</t>
-  </si>
-  <si>
-    <t>DAG-RET-DATE</t>
-  </si>
-  <si>
-    <t>CNT-TERM-TYPE</t>
-  </si>
-  <si>
-    <t>CNT-FINE</t>
-  </si>
-  <si>
-    <t>CNT-TERM-DATE</t>
-  </si>
-  <si>
-    <t>CNT-FIN-MODIFIER</t>
-  </si>
-  <si>
-    <t>PARTY-STATUS</t>
-  </si>
-  <si>
-    <t>APP-DATE</t>
   </si>
   <si>
     <t>/disp-doc:DispositionReport/nc:DocumentIdentification/nc:IdentificationID</t>
@@ -2230,7 +2152,7 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2385,17 +2307,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2430,9 +2343,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2776,13 +2686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:K199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="H76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2792,54 +2702,51 @@
     <col min="3" max="3" width="59" style="1" customWidth="1"/>
     <col min="4" max="4" width="53.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="23" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="35.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="145.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="66.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="145.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="59" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="59" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="31" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="29"/>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>268</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="69"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="31"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="50.25" x14ac:dyDescent="0.25">
+      <c r="F2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="50.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -2849,30 +2756,27 @@
       <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>388</v>
+      <c r="F3" s="27" t="s">
+        <v>144</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="27" t="s">
         <v>153</v>
       </c>
+      <c r="H3" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="I3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="41" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="41" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
@@ -2884,10 +2788,9 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="40"/>
-    </row>
-    <row r="5" spans="1:12" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="10" t="s">
         <v>262</v>
@@ -2895,18 +2798,17 @@
       <c r="C5" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="G5" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="K5" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="10" t="s">
         <v>263</v>
@@ -2914,18 +2816,17 @@
       <c r="C6" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="51" t="s">
+      <c r="F6" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="G6" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="K6" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="10" t="s">
         <v>264</v>
@@ -2933,18 +2834,17 @@
       <c r="C7" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="G7" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="K7" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="10" t="s">
         <v>274</v>
@@ -2952,20 +2852,17 @@
       <c r="C8" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="F8" s="52" t="s">
-        <v>390</v>
-      </c>
-      <c r="G8" s="51" t="s">
+      <c r="F8" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="G8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="K8" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
       <c r="B9" s="10" t="s">
         <v>272</v>
@@ -2973,20 +2870,17 @@
       <c r="C9" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="F9" s="52" t="s">
-        <v>391</v>
-      </c>
-      <c r="G9" s="51" t="s">
+      <c r="F9" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="G9" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="K9" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="10" t="s">
         <v>198</v>
@@ -2994,18 +2888,17 @@
       <c r="C10" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="51" t="s">
+      <c r="F10" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="G10" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="K10" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J10" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="33" t="s">
         <v>227</v>
@@ -3013,18 +2906,17 @@
       <c r="C11" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="51" t="s">
+      <c r="F11" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="G11" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="K11" s="46" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J11" s="46" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="10" t="s">
         <v>275</v>
@@ -3034,21 +2926,20 @@
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="G12" s="33" t="s">
         <v>175</v>
       </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J12" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="10" t="s">
         <v>275</v>
@@ -3056,18 +2947,17 @@
       <c r="C13" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="51" t="s">
+      <c r="F13" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="G13" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="K13" s="22" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J13" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="10" t="s">
         <v>275</v>
@@ -3075,18 +2965,17 @@
       <c r="C14" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="51" t="s">
+      <c r="F14" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="G14" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="K14" s="22" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="10" t="s">
         <v>275</v>
@@ -3094,18 +2983,17 @@
       <c r="C15" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F15" s="52"/>
-      <c r="G15" s="51" t="s">
+      <c r="F15" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="G15" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="K15" s="22" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="33" t="s">
         <v>0</v>
@@ -3116,13 +3004,12 @@
       <c r="E16" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="52"/>
-      <c r="G16" s="51"/>
-      <c r="K16" s="57" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="51"/>
+      <c r="J16" s="54" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="33" t="s">
         <v>2</v>
@@ -3133,11 +3020,10 @@
       <c r="E17" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="K17" s="58"/>
-    </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="51"/>
+      <c r="J17" s="55"/>
+    </row>
+    <row r="18" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>84</v>
       </c>
@@ -3145,14 +3031,13 @@
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="33" t="s">
         <v>7</v>
@@ -3166,20 +3051,17 @@
       <c r="E19" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="52" t="s">
-        <v>397</v>
-      </c>
-      <c r="G19" s="51" t="s">
+      <c r="F19" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="G19" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="K19" s="34" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J19" s="34" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
         <v>8</v>
       </c>
@@ -3192,20 +3074,17 @@
       <c r="E20" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="56" t="s">
-        <v>395</v>
-      </c>
-      <c r="G20" s="51" t="s">
+      <c r="F20" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="G20" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="K20" s="34" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J20" s="34" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="33" t="s">
         <v>9</v>
@@ -3219,18 +3098,17 @@
       <c r="E21" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="51" t="s">
+      <c r="F21" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="G21" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="K21" s="34" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="34" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="33" t="s">
         <v>10</v>
@@ -3244,13 +3122,12 @@
       <c r="E22" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="52"/>
-      <c r="G22" s="51"/>
-      <c r="K22" s="34" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="51"/>
+      <c r="J22" s="34" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="33" t="s">
         <v>86</v>
@@ -3261,13 +3138,12 @@
       <c r="D23" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="51"/>
-      <c r="K23" s="34" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F23" s="51"/>
+      <c r="J23" s="34" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="33" t="s">
         <v>11</v>
@@ -3281,20 +3157,17 @@
       <c r="E24" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" s="46" t="s">
         <v>396</v>
       </c>
-      <c r="G24" s="51" t="s">
-        <v>206</v>
-      </c>
-      <c r="H24" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="33" t="s">
         <v>12</v>
@@ -3305,20 +3178,17 @@
       <c r="E25" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="52" t="s">
-        <v>394</v>
-      </c>
-      <c r="G25" s="51" t="s">
+      <c r="F25" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="G25" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="K25" s="34" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
@@ -3326,14 +3196,13 @@
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="33" t="s">
         <v>13</v>
       </c>
@@ -3343,56 +3212,51 @@
       <c r="E27" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="52"/>
-      <c r="G27" s="51" t="s">
+      <c r="F27" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="G27" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="K27" s="46" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J27" s="46" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="33" t="s">
         <v>273</v>
       </c>
       <c r="C28" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="F28" s="52" t="s">
-        <v>389</v>
-      </c>
-      <c r="G28" s="51" t="s">
+      <c r="F28" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="G28" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="K28" s="46" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J28" s="46" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="33" t="s">
         <v>285</v>
       </c>
       <c r="C29" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="51" t="s">
+      <c r="F29" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="H29" s="33" t="s">
+      <c r="G29" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="K29" s="46" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="46" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="33" t="s">
         <v>133</v>
@@ -3403,13 +3267,12 @@
       <c r="E30" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="52"/>
-      <c r="G30" s="51"/>
-      <c r="K30" s="20" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="51"/>
+      <c r="J30" s="20" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="33" t="s">
         <v>28</v>
@@ -3420,13 +3283,12 @@
       <c r="E31" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="52"/>
-      <c r="G31" s="51"/>
-      <c r="K31" s="34" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F31" s="51"/>
+      <c r="J31" s="34" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>383</v>
       </c>
@@ -3436,20 +3298,17 @@
       <c r="C32" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="F32" s="54" t="s">
-        <v>412</v>
-      </c>
-      <c r="G32" s="35" t="s">
+      <c r="F32" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="G32" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="K32" s="20" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="20" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="35" t="s">
         <v>129</v>
@@ -3460,13 +3319,12 @@
       <c r="E33" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="52"/>
-      <c r="G33" s="51"/>
-      <c r="K33" s="34" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="51"/>
+      <c r="J33" s="34" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
       <c r="B34" s="33" t="s">
         <v>16</v>
@@ -3477,13 +3335,12 @@
       <c r="E34" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="52"/>
-      <c r="G34" s="51"/>
-      <c r="K34" s="34" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="51"/>
+      <c r="J34" s="34" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>139</v>
       </c>
@@ -3496,13 +3353,12 @@
       <c r="E35" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F35" s="52"/>
-      <c r="G35" s="51"/>
-      <c r="K35" s="20" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="51"/>
+      <c r="J35" s="20" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="35" t="s">
         <v>132</v>
@@ -3513,13 +3369,12 @@
       <c r="E36" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="52"/>
-      <c r="G36" s="51"/>
-      <c r="K36" s="20" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="51"/>
+      <c r="J36" s="20" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>40</v>
       </c>
@@ -3532,13 +3387,12 @@
       <c r="E37" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="52"/>
-      <c r="G37" s="51"/>
-      <c r="K37" s="34" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F37" s="51"/>
+      <c r="J37" s="34" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="10" t="s">
         <v>80</v>
@@ -3546,20 +3400,17 @@
       <c r="C38" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="F38" s="52" t="s">
-        <v>404</v>
-      </c>
-      <c r="G38" s="35" t="s">
+      <c r="F38" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="G38" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="K38" s="20" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="20" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>46</v>
       </c>
@@ -3572,13 +3423,12 @@
       <c r="E39" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="52"/>
-      <c r="G39" s="51"/>
-      <c r="K39" s="34" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="51"/>
+      <c r="J39" s="34" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="33" t="s">
         <v>214</v>
@@ -3586,20 +3436,17 @@
       <c r="C40" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="F40" s="52" t="s">
-        <v>406</v>
-      </c>
-      <c r="G40" s="51" t="s">
+      <c r="F40" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="H40" s="33" t="s">
+      <c r="G40" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="K40" s="46" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="46" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>379</v>
       </c>
@@ -3609,18 +3456,17 @@
       <c r="C41" s="33" t="s">
         <v>326</v>
       </c>
-      <c r="F41" s="52"/>
-      <c r="G41" s="51" t="s">
+      <c r="F41" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="H41" s="33" t="s">
+      <c r="G41" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="K41" s="46" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="46" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="10" t="s">
         <v>265</v>
@@ -3628,20 +3474,17 @@
       <c r="C42" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="F42" s="52" t="s">
-        <v>405</v>
-      </c>
-      <c r="G42" s="35" t="s">
+      <c r="F42" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="H42" s="33" t="s">
+      <c r="G42" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="K42" s="20" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="20" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>27</v>
       </c>
@@ -3657,13 +3500,12 @@
       <c r="E43" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="52"/>
-      <c r="G43" s="51"/>
-      <c r="K43" s="34" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="51"/>
+      <c r="J43" s="34" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="33" t="s">
         <v>64</v>
@@ -3677,13 +3519,12 @@
       <c r="E44" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F44" s="52"/>
-      <c r="G44" s="51"/>
-      <c r="K44" s="34" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="51"/>
+      <c r="J44" s="34" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="10" t="s">
         <v>141</v>
@@ -3694,30 +3535,26 @@
       <c r="E45" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="F45" s="52" t="s">
-        <v>392</v>
-      </c>
-      <c r="G45" s="51" t="s">
+      <c r="F45" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="H45" s="33" t="s">
+      <c r="G45" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="K45" s="46" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="10"/>
       <c r="E46" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="52"/>
-      <c r="G46" s="51"/>
-      <c r="K46" s="34"/>
-    </row>
-    <row r="47" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="51"/>
+      <c r="J46" s="34"/>
+    </row>
+    <row r="47" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="10" t="s">
         <v>143</v>
@@ -3728,13 +3565,12 @@
       <c r="E47" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="52"/>
-      <c r="G47" s="51"/>
-      <c r="K47" s="34" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F47" s="51"/>
+      <c r="J47" s="34" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
       <c r="B48" s="33" t="s">
         <v>29</v>
@@ -3745,20 +3581,17 @@
       <c r="E48" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="F48" s="52" t="s">
-        <v>398</v>
-      </c>
-      <c r="G48" s="51" t="s">
+      <c r="F48" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="H48" s="33" t="s">
+      <c r="G48" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="K48" s="34" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J48" s="34" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="33" t="s">
         <v>185</v>
@@ -3766,18 +3599,17 @@
       <c r="C49" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="F49" s="52"/>
-      <c r="G49" s="51" t="s">
+      <c r="F49" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="H49" s="33" t="s">
+      <c r="G49" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="K49" s="46" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J49" s="46" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
       <c r="B50" s="33" t="s">
         <v>30</v>
@@ -3788,20 +3620,17 @@
       <c r="E50" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="52" t="s">
-        <v>400</v>
-      </c>
-      <c r="G50" s="51" t="s">
+      <c r="F50" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="H50" s="33" t="s">
+      <c r="G50" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="K50" s="34" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J50" s="34" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="33" t="s">
         <v>25</v>
@@ -3812,20 +3641,17 @@
       <c r="E51" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="52" t="s">
-        <v>399</v>
-      </c>
-      <c r="G51" s="35" t="s">
+      <c r="F51" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="H51" s="33" t="s">
+      <c r="G51" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="K51" s="46" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J51" s="46" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
       <c r="B52" s="33" t="s">
         <v>26</v>
@@ -3836,20 +3662,17 @@
       <c r="E52" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="52" t="s">
-        <v>401</v>
-      </c>
-      <c r="G52" s="35" t="s">
+      <c r="F52" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="H52" s="33" t="s">
+      <c r="G52" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="K52" s="46" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J52" s="46" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="33" t="s">
         <v>187</v>
@@ -3860,18 +3683,17 @@
       <c r="E53" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="52"/>
-      <c r="G53" s="35" t="s">
+      <c r="F53" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="H53" s="33" t="s">
+      <c r="G53" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="K53" s="46" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="46" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="10" t="s">
         <v>130</v>
@@ -3882,13 +3704,12 @@
       <c r="E54" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="F54" s="52"/>
-      <c r="G54" s="51"/>
-      <c r="K54" s="34" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F54" s="51"/>
+      <c r="J54" s="34" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="10" t="s">
         <v>131</v>
@@ -3896,20 +3717,17 @@
       <c r="C55" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F55" s="52" t="s">
-        <v>411</v>
-      </c>
-      <c r="G55" s="51" t="s">
+      <c r="F55" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="H55" s="33" t="s">
+      <c r="G55" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="K55" s="46" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="46" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="42" t="s">
         <v>31</v>
       </c>
@@ -3922,13 +3740,12 @@
       <c r="E56" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F56" s="52"/>
-      <c r="G56" s="51"/>
-      <c r="K56" s="34" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="51"/>
+      <c r="J56" s="34" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
       <c r="B57" s="33" t="s">
         <v>23</v>
@@ -3939,13 +3756,12 @@
       <c r="E57" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F57" s="52"/>
-      <c r="G57" s="51"/>
-      <c r="K57" s="34" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="51"/>
+      <c r="J57" s="34" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="35" t="s">
         <v>128</v>
@@ -3956,13 +3772,12 @@
       <c r="E58" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="F58" s="52"/>
-      <c r="G58" s="51"/>
-      <c r="K58" s="34" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="51"/>
+      <c r="J58" s="34" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
       <c r="B59" s="33" t="s">
         <v>24</v>
@@ -3973,13 +3788,12 @@
       <c r="E59" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="F59" s="52"/>
-      <c r="G59" s="51"/>
-      <c r="K59" s="34" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F59" s="51"/>
+      <c r="J59" s="34" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
       <c r="B60" s="33" t="s">
         <v>266</v>
@@ -3987,18 +3801,17 @@
       <c r="C60" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="F60" s="52"/>
-      <c r="G60" s="51" t="s">
+      <c r="F60" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="H60" s="49" t="s">
+      <c r="G60" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="K60" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J60" s="46" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="33" t="s">
         <v>31</v>
@@ -4006,20 +3819,17 @@
       <c r="C61" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="F61" s="52" t="s">
-        <v>403</v>
-      </c>
-      <c r="G61" s="35" t="s">
+      <c r="F61" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="H61" s="33" t="s">
+      <c r="G61" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="K61" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J61" s="46" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="42" t="s">
         <v>140</v>
       </c>
@@ -4032,20 +3842,17 @@
       <c r="E62" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="F62" s="52" t="s">
-        <v>402</v>
-      </c>
-      <c r="G62" s="35" t="s">
+      <c r="F62" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="H62" s="33" t="s">
+      <c r="G62" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="K62" s="20" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J62" s="20" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
       <c r="B63" s="10" t="s">
         <v>289</v>
@@ -4053,20 +3860,17 @@
       <c r="C63" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="F63" s="52" t="s">
-        <v>407</v>
-      </c>
-      <c r="G63" s="51" t="s">
+      <c r="F63" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="H63" s="33" t="s">
+      <c r="G63" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="K63" s="46" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J63" s="46" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
       <c r="B64" s="10" t="s">
         <v>356</v>
@@ -4077,23 +3881,21 @@
       <c r="D64" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="F64" s="52"/>
-      <c r="G64" s="51" t="s">
+      <c r="F64" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="H64" s="33" t="s">
+      <c r="G64" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="K64" s="46" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F65" s="52"/>
-      <c r="G65" s="51"/>
-      <c r="K65" s="34"/>
-    </row>
-    <row r="66" spans="1:11" s="33" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="46" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="51"/>
+      <c r="J65" s="34"/>
+    </row>
+    <row r="66" spans="1:10" s="33" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
       <c r="B66" s="10" t="s">
         <v>291</v>
@@ -4101,20 +3903,17 @@
       <c r="C66" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="F66" s="55" t="s">
-        <v>413</v>
-      </c>
-      <c r="G66" s="51" t="s">
+      <c r="F66" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="H66" s="33" t="s">
+      <c r="G66" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="K66" s="46" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="33" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J66" s="46" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" s="33" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
       <c r="B67" s="10" t="s">
         <v>241</v>
@@ -4122,18 +3921,17 @@
       <c r="C67" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="F67" s="52"/>
-      <c r="G67" s="35" t="s">
+      <c r="F67" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="H67" s="49" t="s">
+      <c r="G67" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="K67" s="20" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="20" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="33" t="s">
         <v>21</v>
@@ -4144,13 +3942,12 @@
       <c r="E68" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F68" s="52"/>
-      <c r="G68" s="51"/>
-      <c r="K68" s="20" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="51"/>
+      <c r="J68" s="20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>42</v>
       </c>
@@ -4160,18 +3957,17 @@
       <c r="C69" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="F69" s="52"/>
-      <c r="G69" s="35" t="s">
+      <c r="F69" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="H69" s="49" t="s">
+      <c r="G69" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="K69" s="20" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J69" s="20" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="10" t="s">
         <v>359</v>
@@ -4183,16 +3979,15 @@
       <c r="E70" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="10"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
-      <c r="J70" s="10"/>
-      <c r="K70" s="22" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J70" s="22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="10" t="s">
         <v>363</v>
@@ -4204,16 +3999,15 @@
       <c r="E71" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="F71" s="10"/>
-      <c r="G71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="10"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="22" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J71" s="22" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="10" t="s">
         <v>373</v>
@@ -4225,16 +4019,15 @@
       <c r="E72" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="F72" s="10"/>
-      <c r="G72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="10"/>
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
-      <c r="J72" s="10"/>
-      <c r="K72" s="22" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J72" s="22" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
       <c r="B73" s="10" t="s">
         <v>385</v>
@@ -4242,18 +4035,17 @@
       <c r="C73" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="F73" s="52"/>
-      <c r="G73" s="35" t="s">
+      <c r="F73" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="H73" s="33" t="s">
+      <c r="G73" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="K73" s="20" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J73" s="20" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
       <c r="B74" s="10" t="s">
         <v>256</v>
@@ -4264,30 +4056,26 @@
       <c r="E74" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="F74" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="G74" s="35" t="s">
+      <c r="F74" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="H74" s="33" t="s">
+      <c r="G74" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="K74" s="20" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="47" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J74" s="20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="47" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="28"/>
       <c r="B75" s="10"/>
       <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="35"/>
-      <c r="K75" s="20" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F75" s="35"/>
+      <c r="J75" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="10" t="s">
         <v>87</v>
@@ -4299,38 +4087,36 @@
       <c r="E76" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="22" t="s">
+      <c r="F76" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="H76" s="50" t="s">
+      <c r="G76" s="50" t="s">
         <v>247</v>
       </c>
+      <c r="H76" s="10"/>
       <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="22" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J76" s="22" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B77" s="45" t="s">
         <v>92</v>
       </c>
       <c r="C77" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F77" s="52"/>
-      <c r="G77" s="51" t="s">
+      <c r="F77" s="51" t="s">
         <v>212</v>
       </c>
-      <c r="H77" s="45" t="s">
+      <c r="G77" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="K77" s="46" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J77" s="46" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="28"/>
       <c r="B78" s="10" t="s">
         <v>253</v>
@@ -4338,42 +4124,37 @@
       <c r="C78" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="F78" s="52" t="s">
-        <v>409</v>
-      </c>
-      <c r="G78" s="51" t="s">
+      <c r="F78" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="H78" s="49" t="s">
+      <c r="G78" s="49" t="s">
         <v>254</v>
       </c>
-      <c r="K78" s="46" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J78" s="46" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
         <v>371</v>
       </c>
       <c r="E79" s="47" t="s">
         <v>372</v>
       </c>
-      <c r="F79" s="52"/>
-      <c r="G79" s="51"/>
-      <c r="K79" s="48" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" s="45" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="51"/>
+      <c r="J79" s="48" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="45" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="28"/>
       <c r="B80" s="10"/>
-      <c r="F80" s="52"/>
-      <c r="G80" s="51"/>
-      <c r="K80" s="46" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="51"/>
+      <c r="J80" s="46" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="28"/>
       <c r="B81" s="10" t="s">
         <v>259</v>
@@ -4381,20 +4162,17 @@
       <c r="C81" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="F81" s="52" t="s">
-        <v>410</v>
-      </c>
-      <c r="G81" s="35" t="s">
+      <c r="F81" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="H81" s="33" t="s">
+      <c r="G81" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="K81" s="46" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="46" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="10" t="s">
         <v>43</v>
@@ -4402,18 +4180,17 @@
       <c r="C82" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F82" s="52"/>
-      <c r="G82" s="51"/>
-      <c r="K82" s="20" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F82" s="51"/>
+      <c r="J82" s="20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="C83" s="56" t="s">
+      <c r="C83" s="53" t="s">
         <v>342</v>
       </c>
       <c r="D83" s="33" t="s">
@@ -4422,43 +4199,39 @@
       <c r="E83" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="F83" s="10"/>
-      <c r="G83" s="51"/>
-      <c r="K83" s="58" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F83" s="51"/>
+      <c r="J83" s="55" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="10"/>
-      <c r="C84" s="56"/>
+      <c r="C84" s="53"/>
       <c r="D84" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F84" s="52"/>
-      <c r="G84" s="51"/>
-      <c r="K84" s="58"/>
-    </row>
-    <row r="85" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F84" s="51"/>
+      <c r="J84" s="55"/>
+    </row>
+    <row r="85" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="10"/>
-      <c r="C85" s="56"/>
+      <c r="C85" s="53"/>
       <c r="D85" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="F85" s="52"/>
-      <c r="G85" s="51"/>
-      <c r="K85" s="58"/>
-    </row>
-    <row r="86" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="51"/>
+      <c r="J85" s="55"/>
+    </row>
+    <row r="86" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="10"/>
-      <c r="C86" s="56"/>
+      <c r="C86" s="53"/>
       <c r="D86" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F86" s="52"/>
-      <c r="G86" s="51"/>
-      <c r="K86" s="58"/>
-    </row>
-    <row r="87" spans="1:11" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="51"/>
+      <c r="J86" s="55"/>
+    </row>
+    <row r="87" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>381</v>
       </c>
@@ -4466,14 +4239,13 @@
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="12"/>
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
-      <c r="J87" s="12"/>
-      <c r="K87" s="13"/>
-    </row>
-    <row r="88" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J87" s="13"/>
+    </row>
+    <row r="88" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="33" t="s">
         <v>386</v>
@@ -4481,18 +4253,17 @@
       <c r="C88" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="F88" s="52"/>
-      <c r="G88" s="51" t="s">
+      <c r="F88" s="51" t="s">
         <v>234</v>
       </c>
-      <c r="H88" s="33" t="s">
+      <c r="G88" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="K88" s="20" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J88" s="20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
         <v>382</v>
       </c>
@@ -4502,18 +4273,17 @@
       <c r="C89" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="F89" s="52"/>
-      <c r="G89" s="51" t="s">
+      <c r="F89" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="H89" s="33" t="s">
+      <c r="G89" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="K89" s="46" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="46" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="28"/>
       <c r="B90" s="10" t="s">
         <v>236</v>
@@ -4521,18 +4291,17 @@
       <c r="C90" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="F90" s="52"/>
-      <c r="G90" s="35" t="s">
+      <c r="F90" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="H90" s="33" t="s">
+      <c r="G90" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="K90" s="46" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="46" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
         <v>383</v>
       </c>
@@ -4542,18 +4311,17 @@
       <c r="C91" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="F91" s="52"/>
-      <c r="G91" s="51" t="s">
+      <c r="F91" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="H91" s="49" t="s">
+      <c r="G91" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="K91" s="46" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J91" s="46" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="10" t="s">
         <v>245</v>
@@ -4563,20 +4331,19 @@
       </c>
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="22" t="s">
+      <c r="F92" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="H92" s="50" t="s">
+      <c r="G92" s="50" t="s">
         <v>246</v>
       </c>
+      <c r="H92" s="10"/>
       <c r="I92" s="10"/>
-      <c r="J92" s="10"/>
-      <c r="K92" s="22" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="22" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
         <v>384</v>
       </c>
@@ -4588,20 +4355,19 @@
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="22" t="s">
+      <c r="F93" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="H93" s="10" t="s">
+      <c r="G93" s="10" t="s">
         <v>252</v>
       </c>
+      <c r="H93" s="10"/>
       <c r="I93" s="10"/>
-      <c r="J93" s="10"/>
-      <c r="K93" s="22" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J93" s="22" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="10" t="s">
         <v>250</v>
@@ -4611,20 +4377,19 @@
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="22" t="s">
+      <c r="F94" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="H94" s="10" t="s">
+      <c r="G94" s="10" t="s">
         <v>248</v>
       </c>
+      <c r="H94" s="10"/>
       <c r="I94" s="10"/>
-      <c r="J94" s="10"/>
-      <c r="K94" s="20" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J94" s="20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="10" t="s">
         <v>335</v>
@@ -4634,20 +4399,19 @@
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="53" t="s">
+      <c r="F95" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="H95" s="50" t="s">
+      <c r="G95" s="50" t="s">
         <v>249</v>
       </c>
+      <c r="H95" s="10"/>
       <c r="I95" s="10"/>
-      <c r="J95" s="10"/>
-      <c r="K95" s="22" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J95" s="22" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
         <v>376</v>
       </c>
@@ -4660,12 +4424,12 @@
       <c r="D96" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="G96" s="38"/>
-      <c r="K96" s="38" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F96" s="38"/>
+      <c r="J96" s="38" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="28"/>
       <c r="B97" s="10" t="s">
         <v>267</v>
@@ -4676,13 +4440,12 @@
       <c r="D97" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="F97" s="52"/>
-      <c r="G97" s="51"/>
-      <c r="K97" s="34" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="51"/>
+      <c r="J97" s="34" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
       <c r="B98" s="33" t="s">
         <v>352</v>
@@ -4693,13 +4456,12 @@
       <c r="D98" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="F98" s="52"/>
-      <c r="G98" s="51"/>
-      <c r="K98" s="20" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F98" s="51"/>
+      <c r="J98" s="20" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
       <c r="B99" s="33" t="s">
         <v>190</v>
@@ -4707,18 +4469,17 @@
       <c r="C99" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="F99" s="52"/>
-      <c r="G99" s="51" t="s">
+      <c r="F99" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="H99" s="33" t="s">
+      <c r="G99" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="K99" s="20" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J99" s="20" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="28"/>
       <c r="B100" s="33" t="s">
         <v>350</v>
@@ -4729,13 +4490,12 @@
       <c r="D100" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="F100" s="52"/>
-      <c r="G100" s="51"/>
-      <c r="K100" s="20" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F100" s="51"/>
+      <c r="J100" s="20" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="33" t="s">
         <v>91</v>
@@ -4746,13 +4506,12 @@
       <c r="D101" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F101" s="52"/>
-      <c r="G101" s="51"/>
-      <c r="K101" s="20" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F101" s="51"/>
+      <c r="J101" s="20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="28"/>
       <c r="B102" s="10" t="s">
         <v>329</v>
@@ -4763,13 +4522,12 @@
       <c r="D102" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="F102" s="52"/>
-      <c r="G102" s="51"/>
-      <c r="K102" s="34" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F102" s="51"/>
+      <c r="J102" s="34" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="28"/>
       <c r="B103" s="33" t="s">
         <v>331</v>
@@ -4780,13 +4538,12 @@
       <c r="D103" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="F103" s="52"/>
-      <c r="G103" s="51"/>
-      <c r="K103" s="20" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103" s="51"/>
+      <c r="J103" s="20" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
         <v>42</v>
       </c>
@@ -4799,16 +4556,15 @@
       <c r="D104" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F104" s="52"/>
-      <c r="G104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="10"/>
       <c r="H104" s="10"/>
       <c r="I104" s="10"/>
-      <c r="J104" s="10"/>
-      <c r="K104" s="22" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J104" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="10" t="s">
         <v>359</v>
@@ -4818,16 +4574,15 @@
       </c>
       <c r="D105" s="10"/>
       <c r="E105" s="10"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="10"/>
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
-      <c r="J105" s="10"/>
-      <c r="K105" s="22" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J105" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="10" t="s">
         <v>363</v>
@@ -4837,16 +4592,15 @@
       </c>
       <c r="D106" s="10"/>
       <c r="E106" s="10"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="10"/>
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
-      <c r="J106" s="10"/>
-      <c r="K106" s="22" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J106" s="22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="10" t="s">
         <v>373</v>
@@ -4856,16 +4610,15 @@
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
-      <c r="F107" s="10"/>
-      <c r="G107" s="22"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="10"/>
       <c r="H107" s="10"/>
       <c r="I107" s="10"/>
-      <c r="J107" s="10"/>
-      <c r="K107" s="22" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J107" s="22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="10" t="s">
         <v>367</v>
@@ -4874,16 +4627,15 @@
         <v>368</v>
       </c>
       <c r="D108" s="10"/>
-      <c r="F108" s="52"/>
-      <c r="G108" s="22"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="10"/>
       <c r="H108" s="10"/>
       <c r="I108" s="10"/>
-      <c r="J108" s="10"/>
-      <c r="K108" s="22" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J108" s="22" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="10" t="s">
         <v>42</v>
@@ -4892,16 +4644,15 @@
         <v>370</v>
       </c>
       <c r="D109" s="10"/>
-      <c r="F109" s="52"/>
-      <c r="G109" s="22"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="10"/>
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
-      <c r="J109" s="10"/>
-      <c r="K109" s="22" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J109" s="22" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="10" t="s">
         <v>44</v>
       </c>
@@ -4911,13 +4662,12 @@
       <c r="D110" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="F110" s="52"/>
-      <c r="G110" s="51"/>
-      <c r="K110" s="34" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110" s="51"/>
+      <c r="J110" s="34" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="10" t="s">
         <v>94</v>
       </c>
@@ -4927,26 +4677,24 @@
       <c r="D111" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="F111" s="52"/>
-      <c r="G111" s="51"/>
-      <c r="K111" s="34" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" s="51"/>
+      <c r="J111" s="34" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="10" t="s">
         <v>371</v>
       </c>
       <c r="E112" s="33" t="s">
         <v>372</v>
       </c>
-      <c r="F112" s="52"/>
-      <c r="G112" s="51"/>
-      <c r="K112" s="34" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F112" s="51"/>
+      <c r="J112" s="34" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="33" t="s">
         <v>88</v>
       </c>
@@ -4956,13 +4704,12 @@
       <c r="D113" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="F113" s="52"/>
-      <c r="G113" s="51"/>
-      <c r="K113" s="34" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F113" s="51"/>
+      <c r="J113" s="34" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="33" t="s">
         <v>92</v>
       </c>
@@ -4972,13 +4719,12 @@
       <c r="D114" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="F114" s="52"/>
-      <c r="G114" s="51"/>
-      <c r="K114" s="34" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F114" s="51"/>
+      <c r="J114" s="34" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="28"/>
       <c r="B115" s="33" t="s">
         <v>123</v>
@@ -4989,13 +4735,12 @@
       <c r="D115" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="F115" s="52"/>
-      <c r="G115" s="51"/>
-      <c r="K115" s="34" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F115" s="51"/>
+      <c r="J115" s="34" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116" s="33" t="s">
         <v>89</v>
@@ -5006,11 +4751,10 @@
       <c r="D116" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="F116" s="52"/>
-      <c r="G116" s="51"/>
-      <c r="K116" s="34"/>
-    </row>
-    <row r="117" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F116" s="51"/>
+      <c r="J116" s="34"/>
+    </row>
+    <row r="117" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
       <c r="B117" s="33" t="s">
         <v>93</v>
@@ -5021,13 +4765,12 @@
       <c r="D117" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="F117" s="52"/>
-      <c r="G117" s="51"/>
-      <c r="K117" s="34" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F117" s="51"/>
+      <c r="J117" s="34" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="28"/>
       <c r="B118" s="33" t="s">
         <v>90</v>
@@ -5038,13 +4781,12 @@
       <c r="D118" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="F118" s="52"/>
-      <c r="G118" s="51"/>
-      <c r="K118" s="34" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F118" s="51"/>
+      <c r="J118" s="34" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="28"/>
       <c r="B119" s="33" t="s">
         <v>269</v>
@@ -5055,20 +4797,19 @@
       <c r="D119" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="F119" s="52"/>
-      <c r="G119" s="51"/>
-      <c r="K119" s="34" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F119" s="51"/>
+      <c r="J119" s="34" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="G120" s="13"/>
-      <c r="K120" s="13"/>
-    </row>
-    <row r="121" spans="1:11" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="F120" s="13"/>
+      <c r="J120" s="13"/>
+    </row>
+    <row r="121" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="28"/>
       <c r="B121" s="33" t="s">
         <v>282</v>
@@ -5076,18 +4817,17 @@
       <c r="C121" s="33" t="s">
         <v>318</v>
       </c>
-      <c r="F121" s="52"/>
-      <c r="G121" s="35" t="s">
+      <c r="F121" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="H121" s="33" t="s">
+      <c r="G121" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="K121" s="46" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J121" s="46" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="28"/>
       <c r="B122" s="32" t="s">
         <v>41</v>
@@ -5095,20 +4835,17 @@
       <c r="C122" s="33" t="s">
         <v>318</v>
       </c>
-      <c r="F122" s="52" t="s">
-        <v>393</v>
-      </c>
-      <c r="G122" s="15" t="s">
+      <c r="F122" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="H122" s="33" t="s">
+      <c r="G122" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="K122" s="51" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J122" s="51" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>134</v>
       </c>
@@ -5120,10 +4857,9 @@
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
-      <c r="J123" s="12"/>
-      <c r="K123" s="43"/>
-    </row>
-    <row r="124" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J123" s="43"/>
+    </row>
+    <row r="124" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
         <v>136</v>
       </c>
@@ -5135,10 +4871,9 @@
       <c r="G124" s="10"/>
       <c r="H124" s="10"/>
       <c r="I124" s="10"/>
-      <c r="J124" s="10"/>
-      <c r="K124" s="44"/>
-    </row>
-    <row r="125" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J124" s="44"/>
+    </row>
+    <row r="125" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="22" t="s">
         <v>135</v>
       </c>
@@ -5150,10 +4885,9 @@
       <c r="G125" s="10"/>
       <c r="H125" s="10"/>
       <c r="I125" s="10"/>
-      <c r="J125" s="10"/>
-      <c r="K125" s="44"/>
-    </row>
-    <row r="126" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J125" s="44"/>
+    </row>
+    <row r="126" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="22" t="s">
         <v>137</v>
       </c>
@@ -5165,10 +4899,9 @@
       <c r="G126" s="10"/>
       <c r="H126" s="10"/>
       <c r="I126" s="10"/>
-      <c r="J126" s="10"/>
-      <c r="K126" s="44"/>
-    </row>
-    <row r="127" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J126" s="44"/>
+    </row>
+    <row r="127" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>138</v>
       </c>
@@ -5180,10 +4913,9 @@
       <c r="G127" s="10"/>
       <c r="H127" s="10"/>
       <c r="I127" s="10"/>
-      <c r="J127" s="10"/>
-      <c r="K127" s="44"/>
-    </row>
-    <row r="128" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J127" s="44"/>
+    </row>
+    <row r="128" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="21"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -5193,745 +4925,672 @@
       <c r="G128" s="10"/>
       <c r="H128" s="10"/>
       <c r="I128" s="10"/>
-      <c r="J128" s="10"/>
-      <c r="K128" s="20"/>
-    </row>
-    <row r="129" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="56" t="s">
+      <c r="J128" s="20"/>
+    </row>
+    <row r="129" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B129" s="56"/>
-      <c r="C129" s="56"/>
-      <c r="F129" s="52"/>
-      <c r="K129" s="34"/>
-    </row>
-    <row r="130" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="56"/>
-      <c r="B130" s="56"/>
-      <c r="C130" s="56"/>
-      <c r="F130" s="52"/>
-      <c r="K130" s="34"/>
-    </row>
-    <row r="131" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="56"/>
-      <c r="B131" s="56"/>
-      <c r="C131" s="56"/>
-      <c r="F131" s="52"/>
-      <c r="K131" s="34"/>
-    </row>
-    <row r="132" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="56"/>
-      <c r="B132" s="56"/>
-      <c r="C132" s="56"/>
-      <c r="F132" s="52"/>
-      <c r="K132" s="34"/>
-    </row>
-    <row r="133" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="56"/>
-      <c r="B133" s="56"/>
-      <c r="C133" s="56"/>
-      <c r="F133" s="52"/>
-      <c r="K133" s="34"/>
-    </row>
-    <row r="134" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="56"/>
-      <c r="B134" s="56"/>
-      <c r="C134" s="56"/>
+      <c r="B129" s="53"/>
+      <c r="C129" s="53"/>
+      <c r="J129" s="34"/>
+    </row>
+    <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="53"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="53"/>
+      <c r="J130" s="34"/>
+    </row>
+    <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="53"/>
+      <c r="B131" s="53"/>
+      <c r="C131" s="53"/>
+      <c r="J131" s="34"/>
+    </row>
+    <row r="132" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="53"/>
+      <c r="B132" s="53"/>
+      <c r="C132" s="53"/>
+      <c r="J132" s="34"/>
+    </row>
+    <row r="133" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="53"/>
+      <c r="B133" s="53"/>
+      <c r="C133" s="53"/>
+      <c r="J133" s="34"/>
+    </row>
+    <row r="134" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="53"/>
+      <c r="B134" s="53"/>
+      <c r="C134" s="53"/>
       <c r="D134" s="33"/>
       <c r="E134" s="33"/>
-      <c r="F134" s="52"/>
+      <c r="F134" s="33"/>
       <c r="G134" s="33"/>
       <c r="H134" s="33"/>
       <c r="I134" s="33"/>
-      <c r="J134" s="33"/>
-      <c r="K134" s="34"/>
-    </row>
-    <row r="135" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J134" s="34"/>
+    </row>
+    <row r="135" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="33"/>
       <c r="B135" s="33"/>
       <c r="C135" s="33"/>
       <c r="D135" s="33"/>
       <c r="E135" s="33"/>
-      <c r="F135" s="52"/>
+      <c r="F135" s="33"/>
       <c r="G135" s="33"/>
       <c r="H135" s="33"/>
       <c r="I135" s="33"/>
-      <c r="J135" s="33"/>
-      <c r="K135" s="34"/>
-    </row>
-    <row r="136" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J135" s="34"/>
+    </row>
+    <row r="136" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="33"/>
       <c r="B136" s="33"/>
       <c r="C136" s="33"/>
       <c r="D136" s="33"/>
       <c r="E136" s="33"/>
-      <c r="F136" s="52"/>
+      <c r="F136" s="33"/>
       <c r="G136" s="33"/>
       <c r="H136" s="33"/>
       <c r="I136" s="33"/>
-      <c r="J136" s="33"/>
-      <c r="K136" s="34"/>
-    </row>
-    <row r="137" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J136" s="34"/>
+    </row>
+    <row r="137" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="33"/>
       <c r="B137" s="33"/>
       <c r="C137" s="33"/>
       <c r="D137" s="33"/>
       <c r="E137" s="33"/>
-      <c r="F137" s="52"/>
+      <c r="F137" s="33"/>
       <c r="G137" s="33"/>
       <c r="H137" s="33"/>
       <c r="I137" s="33"/>
-      <c r="J137" s="33"/>
-      <c r="K137" s="34"/>
-    </row>
-    <row r="138" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J137" s="34"/>
+    </row>
+    <row r="138" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="33"/>
       <c r="B138" s="33"/>
       <c r="C138" s="33"/>
       <c r="E138" s="33"/>
-      <c r="F138" s="52"/>
+      <c r="F138" s="33"/>
       <c r="G138" s="33"/>
       <c r="H138" s="33"/>
       <c r="I138" s="33"/>
-      <c r="J138" s="33"/>
-      <c r="K138" s="34"/>
-    </row>
-    <row r="139" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J138" s="34"/>
+    </row>
+    <row r="139" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="33"/>
       <c r="B139" s="33"/>
       <c r="C139" s="33"/>
       <c r="D139" s="33"/>
       <c r="E139" s="33"/>
-      <c r="F139" s="52"/>
+      <c r="F139" s="33"/>
       <c r="G139" s="33"/>
       <c r="H139" s="33"/>
       <c r="I139" s="33"/>
-      <c r="J139" s="33"/>
-      <c r="K139" s="28"/>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J139" s="28"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="30"/>
       <c r="D140" s="16"/>
       <c r="E140" s="4"/>
-      <c r="F140" s="52"/>
+      <c r="H140" s="24"/>
       <c r="I140" s="24"/>
-      <c r="J140" s="24"/>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="30"/>
       <c r="D141" s="16"/>
       <c r="E141" s="4"/>
-      <c r="F141" s="52"/>
+      <c r="H141" s="24"/>
       <c r="I141" s="24"/>
-      <c r="J141" s="24"/>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="4"/>
       <c r="C142" s="30"/>
       <c r="D142" s="16"/>
       <c r="E142" s="4"/>
-      <c r="F142" s="52"/>
+      <c r="H142" s="24"/>
       <c r="I142" s="24"/>
-      <c r="J142" s="24"/>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="4"/>
       <c r="C143" s="30"/>
       <c r="D143" s="16"/>
       <c r="E143" s="4"/>
-      <c r="F143" s="52"/>
+      <c r="H143" s="24"/>
       <c r="I143" s="24"/>
-      <c r="J143" s="24"/>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="4"/>
       <c r="C144" s="30"/>
       <c r="D144" s="16"/>
       <c r="E144" s="4"/>
-      <c r="F144" s="52"/>
+      <c r="H144" s="24"/>
       <c r="I144" s="24"/>
-      <c r="J144" s="24"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="4"/>
       <c r="C145" s="30"/>
       <c r="D145" s="16"/>
       <c r="E145" s="4"/>
-      <c r="F145" s="52"/>
+      <c r="H145" s="24"/>
       <c r="I145" s="24"/>
-      <c r="J145" s="24"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="4"/>
       <c r="C146" s="30"/>
       <c r="D146" s="16"/>
       <c r="E146" s="4"/>
-      <c r="F146" s="52"/>
+      <c r="H146" s="24"/>
       <c r="I146" s="24"/>
-      <c r="J146" s="24"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="4"/>
       <c r="C147" s="30"/>
       <c r="D147" s="16"/>
       <c r="E147" s="4"/>
-      <c r="F147" s="52"/>
+      <c r="H147" s="24"/>
       <c r="I147" s="24"/>
-      <c r="J147" s="24"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="30"/>
       <c r="D148" s="16"/>
       <c r="E148" s="4"/>
-      <c r="F148" s="52"/>
+      <c r="H148" s="24"/>
       <c r="I148" s="24"/>
-      <c r="J148" s="24"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="30"/>
       <c r="D149" s="16"/>
       <c r="E149" s="4"/>
-      <c r="F149" s="52"/>
+      <c r="H149" s="24"/>
       <c r="I149" s="24"/>
-      <c r="J149" s="24"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="30"/>
       <c r="D150" s="16"/>
       <c r="E150" s="4"/>
-      <c r="F150" s="52"/>
+      <c r="H150" s="24"/>
       <c r="I150" s="24"/>
-      <c r="J150" s="24"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="30"/>
       <c r="D151" s="19"/>
       <c r="E151" s="4"/>
-      <c r="F151" s="52"/>
+      <c r="H151" s="24"/>
       <c r="I151" s="24"/>
-      <c r="J151" s="24"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="30"/>
       <c r="D152" s="16"/>
       <c r="E152" s="4"/>
-      <c r="F152" s="52"/>
+      <c r="H152" s="24"/>
       <c r="I152" s="24"/>
-      <c r="J152" s="24"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="30"/>
       <c r="D153" s="16"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="52"/>
+      <c r="H153" s="24"/>
       <c r="I153" s="24"/>
-      <c r="J153" s="24"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="30"/>
       <c r="D154" s="16"/>
       <c r="E154" s="4"/>
-      <c r="F154" s="52"/>
+      <c r="H154" s="24"/>
       <c r="I154" s="24"/>
-      <c r="J154" s="24"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="30"/>
       <c r="D155" s="16"/>
       <c r="E155" s="4"/>
-      <c r="F155" s="52"/>
+      <c r="H155" s="24"/>
       <c r="I155" s="24"/>
-      <c r="J155" s="24"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="30"/>
       <c r="D156" s="16"/>
       <c r="E156" s="4"/>
-      <c r="F156" s="52"/>
+      <c r="H156" s="24"/>
       <c r="I156" s="24"/>
-      <c r="J156" s="24"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="4"/>
       <c r="C157" s="30"/>
       <c r="D157" s="16"/>
       <c r="E157" s="4"/>
-      <c r="F157" s="52"/>
+      <c r="H157" s="24"/>
       <c r="I157" s="24"/>
-      <c r="J157" s="24"/>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="4"/>
       <c r="C158" s="30"/>
       <c r="D158" s="16"/>
       <c r="E158" s="4"/>
-      <c r="F158" s="52"/>
+      <c r="H158" s="24"/>
       <c r="I158" s="24"/>
-      <c r="J158" s="24"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="4"/>
       <c r="C159" s="30"/>
       <c r="D159" s="16"/>
       <c r="E159" s="4"/>
-      <c r="F159" s="52"/>
+      <c r="H159" s="24"/>
       <c r="I159" s="24"/>
-      <c r="J159" s="24"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="4"/>
       <c r="C160" s="30"/>
       <c r="D160" s="16"/>
       <c r="E160" s="4"/>
-      <c r="F160" s="52"/>
+      <c r="H160" s="24"/>
       <c r="I160" s="24"/>
-      <c r="J160" s="24"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="4"/>
       <c r="C161" s="30"/>
       <c r="D161" s="16"/>
       <c r="E161" s="4"/>
-      <c r="F161" s="52"/>
+      <c r="H161" s="24"/>
       <c r="I161" s="24"/>
-      <c r="J161" s="24"/>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="4"/>
       <c r="C162" s="30"/>
       <c r="D162" s="16"/>
       <c r="E162" s="4"/>
-      <c r="F162" s="52"/>
+      <c r="H162" s="24"/>
       <c r="I162" s="24"/>
-      <c r="J162" s="24"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="4"/>
       <c r="C163" s="30"/>
       <c r="D163" s="16"/>
       <c r="E163" s="4"/>
-      <c r="F163" s="52"/>
+      <c r="H163" s="24"/>
       <c r="I163" s="24"/>
-      <c r="J163" s="24"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="4"/>
       <c r="C164" s="30"/>
       <c r="D164" s="16"/>
       <c r="E164" s="4"/>
-      <c r="F164" s="52"/>
+      <c r="H164" s="24"/>
       <c r="I164" s="24"/>
-      <c r="J164" s="24"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="4"/>
       <c r="C165" s="30"/>
       <c r="D165" s="16"/>
       <c r="E165" s="4"/>
-      <c r="F165" s="52"/>
+      <c r="H165" s="24"/>
       <c r="I165" s="24"/>
-      <c r="J165" s="24"/>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="4"/>
       <c r="C166" s="30"/>
       <c r="D166" s="16"/>
       <c r="E166" s="4"/>
-      <c r="F166" s="52"/>
+      <c r="H166" s="24"/>
       <c r="I166" s="24"/>
-      <c r="J166" s="24"/>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="4"/>
       <c r="C167" s="30"/>
       <c r="D167" s="16"/>
       <c r="E167" s="4"/>
-      <c r="F167" s="52"/>
+      <c r="H167" s="24"/>
       <c r="I167" s="24"/>
-      <c r="J167" s="24"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="4"/>
       <c r="C168" s="30"/>
       <c r="D168" s="16"/>
       <c r="E168" s="4"/>
-      <c r="F168" s="52"/>
+      <c r="H168" s="24"/>
       <c r="I168" s="24"/>
-      <c r="J168" s="24"/>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="4"/>
       <c r="C169" s="30"/>
       <c r="D169" s="16"/>
       <c r="E169" s="4"/>
-      <c r="F169" s="52"/>
+      <c r="H169" s="24"/>
       <c r="I169" s="24"/>
-      <c r="J169" s="24"/>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="4"/>
       <c r="C170" s="30"/>
       <c r="D170" s="16"/>
       <c r="E170" s="4"/>
-      <c r="F170" s="52"/>
+      <c r="H170" s="24"/>
       <c r="I170" s="24"/>
-      <c r="J170" s="24"/>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="4"/>
       <c r="C171" s="30"/>
       <c r="D171" s="16"/>
       <c r="E171" s="4"/>
-      <c r="F171" s="52"/>
+      <c r="H171" s="24"/>
       <c r="I171" s="24"/>
-      <c r="J171" s="24"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="4"/>
       <c r="C172" s="30"/>
       <c r="D172" s="16"/>
       <c r="E172" s="4"/>
-      <c r="F172" s="52"/>
+      <c r="H172" s="24"/>
       <c r="I172" s="24"/>
-      <c r="J172" s="24"/>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
       <c r="C173" s="30"/>
       <c r="D173" s="16"/>
       <c r="E173" s="4"/>
-      <c r="F173" s="52"/>
+      <c r="H173" s="24"/>
       <c r="I173" s="24"/>
-      <c r="J173" s="24"/>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="4"/>
       <c r="C174" s="30"/>
       <c r="D174" s="16"/>
       <c r="E174" s="4"/>
-      <c r="F174" s="52"/>
+      <c r="H174" s="24"/>
       <c r="I174" s="24"/>
-      <c r="J174" s="24"/>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="4"/>
       <c r="C175" s="30"/>
       <c r="D175" s="16"/>
       <c r="E175" s="4"/>
-      <c r="F175" s="52"/>
+      <c r="H175" s="24"/>
       <c r="I175" s="24"/>
-      <c r="J175" s="24"/>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="4"/>
       <c r="C176" s="30"/>
       <c r="D176" s="16"/>
       <c r="E176" s="4"/>
-      <c r="F176" s="52"/>
+      <c r="H176" s="24"/>
       <c r="I176" s="24"/>
-      <c r="J176" s="24"/>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="4"/>
       <c r="C177" s="30"/>
       <c r="D177" s="16"/>
       <c r="E177" s="4"/>
-      <c r="F177" s="52"/>
+      <c r="H177" s="24"/>
       <c r="I177" s="24"/>
-      <c r="J177" s="24"/>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="4"/>
       <c r="C178" s="30"/>
       <c r="D178" s="16"/>
       <c r="E178" s="4"/>
-      <c r="F178" s="52"/>
+      <c r="H178" s="24"/>
       <c r="I178" s="24"/>
-      <c r="J178" s="24"/>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="4"/>
       <c r="C179" s="30"/>
       <c r="D179" s="16"/>
       <c r="E179" s="4"/>
-      <c r="F179" s="52"/>
+      <c r="H179" s="24"/>
       <c r="I179" s="24"/>
-      <c r="J179" s="24"/>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="4"/>
       <c r="C180" s="30"/>
       <c r="D180" s="16"/>
       <c r="E180" s="4"/>
-      <c r="F180" s="52"/>
+      <c r="H180" s="24"/>
       <c r="I180" s="24"/>
-      <c r="J180" s="24"/>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="4"/>
       <c r="C181" s="30"/>
       <c r="D181" s="16"/>
       <c r="E181" s="4"/>
-      <c r="F181" s="52"/>
+      <c r="H181" s="24"/>
       <c r="I181" s="24"/>
-      <c r="J181" s="24"/>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="4"/>
       <c r="C182" s="30"/>
       <c r="D182" s="16"/>
       <c r="E182" s="4"/>
-      <c r="F182" s="52"/>
+      <c r="H182" s="24"/>
       <c r="I182" s="24"/>
-      <c r="J182" s="24"/>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="4"/>
       <c r="C183" s="30"/>
       <c r="D183" s="16"/>
       <c r="E183" s="4"/>
-      <c r="F183" s="52"/>
+      <c r="H183" s="24"/>
       <c r="I183" s="24"/>
-      <c r="J183" s="24"/>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="4"/>
       <c r="C184" s="30"/>
       <c r="D184" s="16"/>
       <c r="E184" s="4"/>
-      <c r="F184" s="52"/>
+      <c r="H184" s="24"/>
       <c r="I184" s="24"/>
-      <c r="J184" s="24"/>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="4"/>
       <c r="C185" s="30"/>
       <c r="D185" s="16"/>
       <c r="E185" s="4"/>
-      <c r="F185" s="52"/>
+      <c r="H185" s="24"/>
       <c r="I185" s="24"/>
-      <c r="J185" s="24"/>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="4"/>
       <c r="C186" s="30"/>
       <c r="D186" s="16"/>
       <c r="E186" s="4"/>
-      <c r="F186" s="52"/>
+      <c r="H186" s="24"/>
       <c r="I186" s="24"/>
-      <c r="J186" s="24"/>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="4"/>
       <c r="C187" s="30"/>
       <c r="D187" s="16"/>
       <c r="E187" s="4"/>
-      <c r="F187" s="52"/>
+      <c r="H187" s="24"/>
       <c r="I187" s="24"/>
-      <c r="J187" s="24"/>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="4"/>
       <c r="C188" s="30"/>
       <c r="D188" s="16"/>
       <c r="E188" s="4"/>
-      <c r="F188" s="52"/>
+      <c r="H188" s="24"/>
       <c r="I188" s="24"/>
-      <c r="J188" s="24"/>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="4"/>
       <c r="C189" s="30"/>
       <c r="D189" s="16"/>
       <c r="E189" s="4"/>
-      <c r="F189" s="52"/>
+      <c r="H189" s="24"/>
       <c r="I189" s="24"/>
-      <c r="J189" s="24"/>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="4"/>
       <c r="C190" s="30"/>
       <c r="D190" s="16"/>
       <c r="E190" s="4"/>
-      <c r="F190" s="52"/>
+      <c r="H190" s="24"/>
       <c r="I190" s="24"/>
-      <c r="J190" s="24"/>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="4"/>
       <c r="C191" s="30"/>
       <c r="D191" s="16"/>
       <c r="E191" s="4"/>
-      <c r="F191" s="52"/>
+      <c r="H191" s="24"/>
       <c r="I191" s="24"/>
-      <c r="J191" s="24"/>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="4"/>
       <c r="C192" s="30"/>
       <c r="D192" s="16"/>
       <c r="E192" s="4"/>
-      <c r="F192" s="52"/>
+      <c r="H192" s="24"/>
       <c r="I192" s="24"/>
-      <c r="J192" s="24"/>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="4"/>
       <c r="C193" s="30"/>
       <c r="D193" s="16"/>
       <c r="E193" s="4"/>
-      <c r="F193" s="52"/>
+      <c r="H193" s="24"/>
       <c r="I193" s="24"/>
-      <c r="J193" s="24"/>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="4"/>
       <c r="C194" s="30"/>
       <c r="D194" s="16"/>
       <c r="E194" s="4"/>
-      <c r="F194" s="52"/>
+      <c r="H194" s="24"/>
       <c r="I194" s="24"/>
-      <c r="J194" s="24"/>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="4"/>
       <c r="C195" s="30"/>
       <c r="D195" s="16"/>
       <c r="E195" s="4"/>
-      <c r="F195" s="52"/>
+      <c r="H195" s="24"/>
       <c r="I195" s="24"/>
-      <c r="J195" s="24"/>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="4"/>
       <c r="C196" s="30"/>
       <c r="D196" s="16"/>
       <c r="E196" s="4"/>
-      <c r="F196" s="52"/>
+      <c r="H196" s="24"/>
       <c r="I196" s="24"/>
-      <c r="J196" s="24"/>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="4"/>
       <c r="C197" s="30"/>
       <c r="D197" s="16"/>
       <c r="E197" s="4"/>
-      <c r="F197" s="52"/>
+      <c r="H197" s="24"/>
       <c r="I197" s="24"/>
-      <c r="J197" s="24"/>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="4"/>
       <c r="C198" s="30"/>
       <c r="D198" s="16"/>
       <c r="E198" s="4"/>
-      <c r="F198" s="52"/>
+      <c r="H198" s="24"/>
       <c r="I198" s="24"/>
-      <c r="J198" s="24"/>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="4"/>
       <c r="C199" s="30"/>
       <c r="D199" s="16"/>
       <c r="E199" s="4"/>
-      <c r="F199" s="52"/>
+      <c r="H199" s="24"/>
       <c r="I199" s="24"/>
-      <c r="J199" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A129:C134"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="K83:K86"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J83:J86"/>
     <mergeCell ref="C83:C86"/>
-    <mergeCell ref="F20:F21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H69" r:id="rId1"/>
-    <hyperlink ref="H78" r:id="rId2"/>
-    <hyperlink ref="H92" r:id="rId3"/>
-    <hyperlink ref="H91" r:id="rId4"/>
-    <hyperlink ref="H67" r:id="rId5"/>
-    <hyperlink ref="H60" r:id="rId6"/>
-    <hyperlink ref="H76" r:id="rId7"/>
-    <hyperlink ref="H95" r:id="rId8"/>
+    <hyperlink ref="G69" r:id="rId1"/>
+    <hyperlink ref="G78" r:id="rId2"/>
+    <hyperlink ref="G92" r:id="rId3"/>
+    <hyperlink ref="G91" r:id="rId4"/>
+    <hyperlink ref="G67" r:id="rId5"/>
+    <hyperlink ref="G60" r:id="rId6"/>
+    <hyperlink ref="G76" r:id="rId7"/>
+    <hyperlink ref="G95" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>

</xml_diff>

<commit_message>
Added RegisteredOffenderIdentficaton to the IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="480">
   <si>
     <t>Submitted Date</t>
   </si>
@@ -568,9 +568,6 @@
     <t>/OBTSBATCHTRANSACTION/OBTSLOGICALTRANSACTION/@CHARGEOTN</t>
   </si>
   <si>
-    <t>CHARGEARN</t>
-  </si>
-  <si>
     <t>/OBTSBATCHTRANSACTION/OBTSLOGICALTRANSACTION/@CHARGEARN</t>
   </si>
   <si>
@@ -1232,9 +1229,6 @@
     <t>/disp-doc:DispositionReport/nc:DocumentIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/disp-doc:DispositionReport/nc:DocumentSource/nc:EntityOrganization/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/disp-doc:DispositionReport/cyfs:SubmittedDateTime/nc:DateTime</t>
   </si>
   <si>
@@ -1497,6 +1491,18 @@
   </si>
   <si>
     <t>/disp-doc:DispositionReport/j:Charge/j:ChargeSentence/disp-ext:SentenceAugmentation/j:SentenceTerm/disp-ext:SentenceTermAugmentation/disp-ext:SentenceSuspendedTimeRemainder</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/j:Subject/disp-ext:SubjectAugmentation/j:RegisteredOffender/j:RegisteredOffenderIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>CHG_ARN</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/ext:DocumentOtherIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/dr:DispositionReports/exchange:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCourt/nc:OrganizationIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2158,7 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2308,6 +2314,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2689,10 +2701,10 @@
   <dimension ref="A1:K199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="H76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="J28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F1:F1048576"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,21 +2723,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="56" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="57"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="31" t="s">
         <v>82</v>
       </c>
@@ -2734,14 +2746,14 @@
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="29"/>
-      <c r="D2" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="63" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="25"/>
       <c r="I2" s="26"/>
       <c r="J2" s="31"/>
@@ -2756,9 +2768,9 @@
       <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="64"/>
       <c r="E3" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>144</v>
@@ -2793,205 +2805,189 @@
     <row r="5" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="46" t="s">
-        <v>388</v>
-      </c>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J6" s="46" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F7" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>181</v>
-      </c>
       <c r="J7" s="46" t="s">
-        <v>388</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="46" t="s">
-        <v>388</v>
-      </c>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
       <c r="B9" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F9" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="J9" s="46" t="s">
-        <v>388</v>
-      </c>
+      <c r="J9" s="46"/>
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>301</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="J10" s="46" t="s">
-        <v>388</v>
-      </c>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="F11" s="51" t="s">
+      <c r="G11" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="G11" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="J11" s="46" t="s">
-        <v>388</v>
+      <c r="J11" s="54" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>275</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>276</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="22" t="s">
-        <v>389</v>
-      </c>
+      <c r="J12" s="22"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>276</v>
-      </c>
       <c r="F13" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>389</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>276</v>
-      </c>
       <c r="F14" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>389</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:11" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>276</v>
-      </c>
       <c r="F15" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>389</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:11" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
@@ -3005,8 +3001,8 @@
         <v>47</v>
       </c>
       <c r="F16" s="51"/>
-      <c r="J16" s="54" t="s">
-        <v>390</v>
+      <c r="J16" s="56" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3021,7 +3017,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="51"/>
-      <c r="J17" s="55"/>
+      <c r="J17" s="57"/>
     </row>
     <row r="18" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -3043,7 +3039,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>99</v>
@@ -3052,13 +3048,13 @@
         <v>49</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>146</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3066,7 +3062,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D20" s="33" t="s">
         <v>100</v>
@@ -3081,7 +3077,7 @@
         <v>169</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3090,7 +3086,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>101</v>
@@ -3105,7 +3101,7 @@
         <v>168</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3114,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" s="33" t="s">
         <v>102</v>
@@ -3124,7 +3120,7 @@
       </c>
       <c r="F22" s="51"/>
       <c r="J22" s="34" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3133,14 +3129,14 @@
         <v>86</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D23" s="33" t="s">
         <v>103</v>
       </c>
       <c r="F23" s="51"/>
       <c r="J23" s="34" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3149,7 +3145,7 @@
         <v>11</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D24" s="33" t="s">
         <v>104</v>
@@ -3158,13 +3154,13 @@
         <v>53</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G24" s="33" t="s">
         <v>147</v>
       </c>
       <c r="J24" s="46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3173,386 +3169,388 @@
         <v>12</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G25" s="33" t="s">
         <v>148</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="10"/>
+      <c r="E26" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="51"/>
+      <c r="J26" s="53" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="J27" s="46" t="s">
-        <v>398</v>
-      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="33" t="s">
-        <v>273</v>
+        <v>13</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>271</v>
+        <v>283</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>57</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="J28" s="46" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F29" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="J29" s="46" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="C29" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="F29" s="51" t="s">
+      <c r="F30" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="G30" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="G29" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="J29" s="46" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="51"/>
-      <c r="J30" s="20" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="46" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="51"/>
+      <c r="J31" s="20" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="E31" s="33" t="s">
+      <c r="C32" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="E32" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="51"/>
-      <c r="J31" s="34" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
-        <v>383</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>377</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="51"/>
+      <c r="J32" s="34" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="G33" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="35" t="s">
+      <c r="J33" s="20" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="E33" s="33" t="s">
+      <c r="C34" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>62</v>
-      </c>
-      <c r="F33" s="51"/>
-      <c r="J33" s="34" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>63</v>
       </c>
       <c r="F34" s="51"/>
       <c r="J34" s="34" t="s">
-        <v>400</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="28"/>
+      <c r="B35" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="51"/>
+      <c r="J35" s="34" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B36" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="E35" s="33" t="s">
+      <c r="C36" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="E36" s="33" t="s">
         <v>55</v>
-      </c>
-      <c r="F35" s="51"/>
-      <c r="J35" s="20" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>56</v>
       </c>
       <c r="F36" s="51"/>
       <c r="J36" s="20" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="51"/>
+      <c r="J37" s="20" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="51"/>
+      <c r="J38" s="34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="51"/>
+      <c r="J40" s="34" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="F41" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J41" s="46" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="F42" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J42" s="46" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" s="20" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="E37" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" s="51"/>
-      <c r="J37" s="34" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="J38" s="20" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="E39" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="51"/>
-      <c r="J39" s="34" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="F40" s="51" t="s">
-        <v>215</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="J40" s="46" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>379</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>326</v>
-      </c>
-      <c r="F41" s="51" t="s">
-        <v>239</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="J41" s="46" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>327</v>
-      </c>
-      <c r="F42" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="G42" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="J42" s="20" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+    <row r="44" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B44" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C44" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D44" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E44" s="33" t="s">
         <v>66</v>
-      </c>
-      <c r="F43" s="51"/>
-      <c r="J43" s="34" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>374</v>
-      </c>
-      <c r="D44" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E44" s="33" t="s">
-        <v>67</v>
       </c>
       <c r="F44" s="51"/>
       <c r="J44" s="34" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="51"/>
+      <c r="J45" s="34" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
+      <c r="B46" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="E45" s="33" t="s">
+      <c r="C46" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E46" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="F45" s="51" t="s">
+      <c r="F46" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="G45" s="33" t="s">
+      <c r="G46" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="J45" s="46" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="10"/>
-      <c r="E46" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="51"/>
-      <c r="J46" s="34"/>
+      <c r="J46" s="46" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="47" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
@@ -3560,14 +3558,14 @@
         <v>143</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>65</v>
       </c>
       <c r="F47" s="51"/>
       <c r="J47" s="34" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3576,37 +3574,37 @@
         <v>29</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E48" s="33" t="s">
         <v>68</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G48" s="33" t="s">
         <v>158</v>
       </c>
       <c r="J48" s="34" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F49" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="G49" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="G49" s="33" t="s">
-        <v>184</v>
-      </c>
       <c r="J49" s="46" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3615,19 +3613,19 @@
         <v>30</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E50" s="33" t="s">
         <v>69</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G50" s="33" t="s">
         <v>156</v>
       </c>
       <c r="J50" s="34" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3636,19 +3634,19 @@
         <v>25</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E51" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F51" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G51" s="33" t="s">
         <v>159</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3657,40 +3655,40 @@
         <v>26</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E52" s="33" t="s">
         <v>71</v>
       </c>
       <c r="F52" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G52" s="33" t="s">
         <v>157</v>
       </c>
       <c r="J52" s="46" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E53" s="33" t="s">
         <v>69</v>
       </c>
       <c r="F53" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="G53" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="G53" s="33" t="s">
-        <v>189</v>
-      </c>
       <c r="J53" s="46" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3706,7 +3704,7 @@
       </c>
       <c r="F54" s="51"/>
       <c r="J54" s="34" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3718,13 +3716,13 @@
         <v>83</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G55" s="33" t="s">
         <v>160</v>
       </c>
       <c r="J55" s="46" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3742,7 +3740,7 @@
       </c>
       <c r="F56" s="51"/>
       <c r="J56" s="34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3758,7 +3756,7 @@
       </c>
       <c r="F57" s="51"/>
       <c r="J57" s="34" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3774,7 +3772,7 @@
       </c>
       <c r="F58" s="51"/>
       <c r="J58" s="34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3790,25 +3788,25 @@
       </c>
       <c r="F59" s="51"/>
       <c r="J59" s="34" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
       <c r="B60" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G60" s="49" t="s">
         <v>162</v>
       </c>
       <c r="J60" s="46" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3817,16 +3815,16 @@
         <v>31</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F61" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G61" s="33" t="s">
         <v>161</v>
       </c>
       <c r="J61" s="46" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3837,58 +3835,58 @@
         <v>140</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E62" s="33" t="s">
         <v>77</v>
       </c>
       <c r="F62" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G62" s="33" t="s">
         <v>163</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
       <c r="B63" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F63" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="G63" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="G63" s="33" t="s">
-        <v>233</v>
-      </c>
       <c r="J63" s="46" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
       <c r="B64" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D64" s="33" t="s">
         <v>112</v>
       </c>
       <c r="F64" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G64" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J64" s="46" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -3898,37 +3896,37 @@
     <row r="66" spans="1:10" s="33" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
       <c r="B66" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C66" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="C66" s="33" t="s">
-        <v>292</v>
-      </c>
       <c r="F66" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G66" s="33" t="s">
         <v>165</v>
       </c>
       <c r="J66" s="46" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="33" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
       <c r="B67" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F67" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G67" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="G67" s="49" t="s">
-        <v>201</v>
-      </c>
       <c r="J67" s="20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3937,14 +3935,14 @@
         <v>21</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E68" s="33" t="s">
         <v>78</v>
       </c>
       <c r="F68" s="51"/>
       <c r="J68" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3952,118 +3950,118 @@
         <v>42</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F69" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G69" s="49" t="s">
         <v>166</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="70" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="D70" s="10"/>
       <c r="E70" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F70" s="22"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>363</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>364</v>
       </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="22" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>373</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>374</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F72" s="22"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
       <c r="J72" s="22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="28"/>
       <c r="B73" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F73" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G73" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J73" s="20" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
       <c r="B74" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F74" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="C74" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="F74" s="35" t="s">
+      <c r="G74" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="G74" s="33" t="s">
-        <v>258</v>
-      </c>
       <c r="J74" s="20" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="47" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4072,7 +4070,7 @@
       <c r="E75" s="10"/>
       <c r="F75" s="35"/>
       <c r="J75" s="20" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -4081,22 +4079,22 @@
         <v>87</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F76" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G76" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4104,46 +4102,46 @@
         <v>92</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F77" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G77" s="45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J77" s="46" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="28"/>
       <c r="B78" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="F78" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="G78" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="C78" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="F78" s="51" t="s">
-        <v>255</v>
-      </c>
-      <c r="G78" s="49" t="s">
-        <v>254</v>
-      </c>
       <c r="J78" s="46" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E79" s="47" t="s">
         <v>371</v>
-      </c>
-      <c r="E79" s="47" t="s">
-        <v>372</v>
       </c>
       <c r="F79" s="51"/>
       <c r="J79" s="48" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="45" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -4151,25 +4149,25 @@
       <c r="B80" s="10"/>
       <c r="F80" s="51"/>
       <c r="J80" s="46" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="28"/>
       <c r="B81" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F81" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="C81" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="F81" s="35" t="s">
+      <c r="G81" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="G81" s="33" t="s">
-        <v>261</v>
-      </c>
       <c r="J81" s="46" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,58 +4180,58 @@
       </c>
       <c r="F82" s="51"/>
       <c r="J82" s="20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="C83" s="53" t="s">
-        <v>342</v>
+        <v>386</v>
+      </c>
+      <c r="C83" s="55" t="s">
+        <v>341</v>
       </c>
       <c r="D83" s="33" t="s">
         <v>117</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F83" s="51"/>
-      <c r="J83" s="55" t="s">
-        <v>418</v>
+      <c r="J83" s="57" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="10"/>
-      <c r="C84" s="53"/>
+      <c r="C84" s="55"/>
       <c r="D84" s="33" t="s">
         <v>96</v>
       </c>
       <c r="F84" s="51"/>
-      <c r="J84" s="55"/>
+      <c r="J84" s="57"/>
     </row>
     <row r="85" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="10"/>
-      <c r="C85" s="53"/>
+      <c r="C85" s="55"/>
       <c r="D85" s="33" t="s">
         <v>97</v>
       </c>
       <c r="F85" s="51"/>
-      <c r="J85" s="55"/>
+      <c r="J85" s="57"/>
     </row>
     <row r="86" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="10"/>
-      <c r="C86" s="53"/>
+      <c r="C86" s="55"/>
       <c r="D86" s="33" t="s">
         <v>98</v>
       </c>
       <c r="F86" s="51"/>
-      <c r="J86" s="55"/>
+      <c r="J86" s="57"/>
     </row>
     <row r="87" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
@@ -4248,251 +4246,251 @@
     <row r="88" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="33" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F88" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="G88" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="G88" s="33" t="s">
-        <v>235</v>
-      </c>
       <c r="J88" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="89" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F89" s="51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G89" s="33" t="s">
         <v>164</v>
       </c>
       <c r="J89" s="46" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="90" spans="1:10" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="28"/>
       <c r="B90" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C90" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="F90" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="C90" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="F90" s="35" t="s">
+      <c r="G90" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="G90" s="33" t="s">
-        <v>238</v>
-      </c>
       <c r="J90" s="46" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F91" s="51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G91" s="49" t="s">
         <v>152</v>
       </c>
       <c r="J91" s="46" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="92" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
       <c r="F92" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G92" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H92" s="10"/>
       <c r="I92" s="10"/>
       <c r="J92" s="22" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
       <c r="F93" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H93" s="10"/>
       <c r="I93" s="10"/>
       <c r="J93" s="22" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="94" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
       <c r="F94" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
       <c r="J94" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C95" s="10" t="s">
         <v>335</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>336</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
       <c r="F95" s="52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G95" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
       <c r="J95" s="22" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B96" s="37" t="s">
         <v>95</v>
       </c>
       <c r="C96" s="37" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D96" s="37" t="s">
         <v>108</v>
       </c>
       <c r="F96" s="38"/>
       <c r="J96" s="38" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="28"/>
       <c r="B97" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D97" s="33" t="s">
         <v>107</v>
       </c>
       <c r="F97" s="51"/>
       <c r="J97" s="34" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="98" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="15"/>
       <c r="B98" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D98" s="33" t="s">
         <v>109</v>
       </c>
       <c r="F98" s="51"/>
       <c r="J98" s="20" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="99" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="15"/>
       <c r="B99" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="F99" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="C99" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="F99" s="51" t="s">
+      <c r="G99" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="G99" s="33" t="s">
-        <v>192</v>
-      </c>
       <c r="J99" s="20" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="28"/>
       <c r="B100" s="33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C100" s="33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D100" s="33" t="s">
         <v>110</v>
       </c>
       <c r="F100" s="51"/>
       <c r="J100" s="20" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="101" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4501,46 +4499,46 @@
         <v>91</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D101" s="33" t="s">
         <v>111</v>
       </c>
       <c r="F101" s="51"/>
       <c r="J101" s="20" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="102" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="28"/>
       <c r="B102" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D102" s="33" t="s">
         <v>113</v>
       </c>
       <c r="F102" s="51"/>
       <c r="J102" s="34" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="103" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="28"/>
       <c r="B103" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="C103" s="33" t="s">
         <v>331</v>
-      </c>
-      <c r="C103" s="33" t="s">
-        <v>332</v>
       </c>
       <c r="D103" s="33" t="s">
         <v>114</v>
       </c>
       <c r="F103" s="51"/>
       <c r="J103" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="104" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -4551,7 +4549,7 @@
         <v>87</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>115</v>
@@ -4561,16 +4559,16 @@
       <c r="H104" s="10"/>
       <c r="I104" s="10"/>
       <c r="J104" s="22" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="105" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C105" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="D105" s="10"/>
       <c r="E105" s="10"/>
@@ -4579,16 +4577,16 @@
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
       <c r="J105" s="22" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C106" s="10" t="s">
         <v>363</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>364</v>
       </c>
       <c r="D106" s="10"/>
       <c r="E106" s="10"/>
@@ -4597,16 +4595,16 @@
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
       <c r="J106" s="22" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C107" s="10" t="s">
         <v>373</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>374</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
@@ -4615,16 +4613,16 @@
       <c r="H107" s="10"/>
       <c r="I107" s="10"/>
       <c r="J107" s="22" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="108" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="C108" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="D108" s="10"/>
       <c r="F108" s="22"/>
@@ -4632,7 +4630,7 @@
       <c r="H108" s="10"/>
       <c r="I108" s="10"/>
       <c r="J108" s="22" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="109" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -4641,7 +4639,7 @@
         <v>42</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D109" s="10"/>
       <c r="F109" s="22"/>
@@ -4649,7 +4647,7 @@
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
       <c r="J109" s="22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="110" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4657,14 +4655,14 @@
         <v>44</v>
       </c>
       <c r="C110" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D110" s="33" t="s">
         <v>116</v>
       </c>
       <c r="F110" s="51"/>
       <c r="J110" s="34" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="111" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4672,26 +4670,26 @@
         <v>94</v>
       </c>
       <c r="C111" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D111" s="33" t="s">
         <v>120</v>
       </c>
       <c r="F111" s="51"/>
       <c r="J111" s="34" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="112" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E112" s="33" t="s">
         <v>371</v>
-      </c>
-      <c r="E112" s="33" t="s">
-        <v>372</v>
       </c>
       <c r="F112" s="51"/>
       <c r="J112" s="34" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4699,14 +4697,14 @@
         <v>88</v>
       </c>
       <c r="C113" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D113" s="33" t="s">
         <v>119</v>
       </c>
       <c r="F113" s="51"/>
       <c r="J113" s="34" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="114" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4714,14 +4712,14 @@
         <v>92</v>
       </c>
       <c r="C114" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D114" s="33" t="s">
         <v>121</v>
       </c>
       <c r="F114" s="51"/>
       <c r="J114" s="34" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="115" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4730,14 +4728,14 @@
         <v>123</v>
       </c>
       <c r="C115" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D115" s="33" t="s">
         <v>122</v>
       </c>
       <c r="F115" s="51"/>
       <c r="J115" s="34" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="116" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4746,7 +4744,7 @@
         <v>89</v>
       </c>
       <c r="C116" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D116" s="33" t="s">
         <v>125</v>
@@ -4760,14 +4758,14 @@
         <v>93</v>
       </c>
       <c r="C117" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D117" s="33" t="s">
         <v>124</v>
       </c>
       <c r="F117" s="51"/>
       <c r="J117" s="34" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="118" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4776,35 +4774,35 @@
         <v>90</v>
       </c>
       <c r="C118" s="33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D118" s="33" t="s">
         <v>118</v>
       </c>
       <c r="F118" s="51"/>
       <c r="J118" s="34" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="119" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="28"/>
       <c r="B119" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="D119" s="33" t="s">
         <v>269</v>
-      </c>
-      <c r="C119" s="33" t="s">
-        <v>348</v>
-      </c>
-      <c r="D119" s="33" t="s">
-        <v>270</v>
       </c>
       <c r="F119" s="51"/>
       <c r="J119" s="34" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="120" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F120" s="13"/>
       <c r="J120" s="13"/>
@@ -4812,19 +4810,19 @@
     <row r="121" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="28"/>
       <c r="B121" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C121" s="33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F121" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="G121" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="G121" s="33" t="s">
-        <v>195</v>
-      </c>
       <c r="J121" s="46" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="122" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -4833,16 +4831,16 @@
         <v>41</v>
       </c>
       <c r="C122" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="F122" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="F122" s="35" t="s">
+        <v>477</v>
+      </c>
+      <c r="G122" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="G122" s="33" t="s">
-        <v>174</v>
-      </c>
       <c r="J122" s="51" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="123" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -4928,41 +4926,41 @@
       <c r="J128" s="20"/>
     </row>
     <row r="129" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="53" t="s">
+      <c r="A129" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="B129" s="53"/>
-      <c r="C129" s="53"/>
+      <c r="B129" s="55"/>
+      <c r="C129" s="55"/>
       <c r="J129" s="34"/>
     </row>
     <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="53"/>
-      <c r="B130" s="53"/>
-      <c r="C130" s="53"/>
+      <c r="A130" s="55"/>
+      <c r="B130" s="55"/>
+      <c r="C130" s="55"/>
       <c r="J130" s="34"/>
     </row>
     <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="53"/>
-      <c r="B131" s="53"/>
-      <c r="C131" s="53"/>
+      <c r="A131" s="55"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="55"/>
       <c r="J131" s="34"/>
     </row>
     <row r="132" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="53"/>
-      <c r="B132" s="53"/>
-      <c r="C132" s="53"/>
+      <c r="A132" s="55"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
       <c r="J132" s="34"/>
     </row>
     <row r="133" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="53"/>
-      <c r="B133" s="53"/>
-      <c r="C133" s="53"/>
+      <c r="A133" s="55"/>
+      <c r="B133" s="55"/>
+      <c r="C133" s="55"/>
       <c r="J133" s="34"/>
     </row>
     <row r="134" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="53"/>
-      <c r="B134" s="53"/>
-      <c r="C134" s="53"/>
+      <c r="A134" s="55"/>
+      <c r="B134" s="55"/>
+      <c r="C134" s="55"/>
       <c r="D134" s="33"/>
       <c r="E134" s="33"/>
       <c r="F134" s="33"/>

</xml_diff>

<commit_message>
Updated mapping spreadsheet for JIMS reporting modifications.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/disposition_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="489">
   <si>
     <t>Submitted Date</t>
   </si>
@@ -1256,9 +1256,6 @@
     <t>/disp-doc:DispositionReport/nc:Case/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/disp-doc:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseOtherIdentification/nc:IdentificationCategoryText</t>
-  </si>
-  <si>
     <t>/disp-doc:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCourtEvent/nc:ActivityDate/nc:Date</t>
   </si>
   <si>
@@ -1503,6 +1500,36 @@
   </si>
   <si>
     <t>/dr:DispositionReports/exchange:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCourt/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Registered Offender</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/j:Charge/j:ChargeSentence/j:SentenceSuspendedIndicator</t>
+  </si>
+  <si>
+    <t>/Recordset/Person/Sentence/Suspended</t>
+  </si>
+  <si>
+    <t>Suspended Sentence</t>
+  </si>
+  <si>
+    <t>Alias Identity</t>
+  </si>
+  <si>
+    <t>/Recordset/Person/PersonAlias</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/nc:Identity</t>
+  </si>
+  <si>
+    <t>ALIAS</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseCourt/nc:OrganizationLocation/nc:Address/nc:LocationCountyName</t>
+  </si>
+  <si>
+    <t>/disp-doc:DispositionReport/nc:Case/j:CaseAugmentation/j:CaseOtherIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2185,7 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2317,6 +2344,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2698,13 +2731,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K199"/>
+  <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="J28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="J64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,21 +2756,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="58" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="58" t="s">
+      <c r="E1" s="67"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="61"/>
       <c r="J1" s="31" t="s">
         <v>82</v>
       </c>
@@ -2746,14 +2779,14 @@
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="29"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="69"/>
       <c r="H2" s="25"/>
       <c r="I2" s="26"/>
       <c r="J2" s="31"/>
@@ -2768,7 +2801,7 @@
       <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="7" t="s">
         <v>357</v>
       </c>
@@ -2851,7 +2884,7 @@
         <v>180</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2917,7 +2950,7 @@
         <v>228</v>
       </c>
       <c r="J11" s="54" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3001,7 +3034,7 @@
         <v>47</v>
       </c>
       <c r="F16" s="51"/>
-      <c r="J16" s="56" t="s">
+      <c r="J16" s="58" t="s">
         <v>388</v>
       </c>
     </row>
@@ -3017,7 +3050,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="51"/>
-      <c r="J17" s="57"/>
+      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -3186,18 +3219,20 @@
     </row>
     <row r="26" spans="1:10" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
-      <c r="B26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>479</v>
+      </c>
       <c r="E26" s="33" t="s">
         <v>79</v>
       </c>
       <c r="F26" s="51"/>
       <c r="J26" s="53" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>22</v>
+        <v>486</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -3209,1402 +3244,1393 @@
       <c r="I27" s="12"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="J28" s="46" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="F29" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="J29" s="46" t="s">
-        <v>397</v>
-      </c>
+    <row r="28" spans="1:10" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>484</v>
+      </c>
+      <c r="F28" s="56"/>
+      <c r="J28" s="56" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
     </row>
     <row r="30" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="J30" s="46" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F31" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="J31" s="56" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C32" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="F30" s="51" t="s">
+      <c r="F32" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="G30" s="33" t="s">
+      <c r="G32" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="J30" s="46" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="33" t="s">
+      <c r="J32" s="56" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="33" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C33" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E33" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="51"/>
-      <c r="J31" s="20" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="33" t="s">
+      <c r="F33" s="51"/>
+      <c r="J33" s="20" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C34" s="33" t="s">
         <v>310</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E34" s="33" t="s">
         <v>58</v>
-      </c>
-      <c r="F32" s="51"/>
-      <c r="J32" s="34" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
-        <v>382</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="G33" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>62</v>
       </c>
       <c r="F34" s="51"/>
       <c r="J34" s="34" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="J35" s="20" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="51"/>
+      <c r="J36" s="34" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" s="51"/>
+      <c r="J37" s="34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="51"/>
+      <c r="J38" s="20" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="51"/>
-      <c r="J35" s="34" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="E36" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="51"/>
-      <c r="J36" s="20" t="s">
+    <row r="39" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="J39" s="20" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="E37" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="51"/>
-      <c r="J37" s="20" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+    <row r="40" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C40" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E40" s="33" t="s">
         <v>59</v>
-      </c>
-      <c r="F38" s="51"/>
-      <c r="J38" s="34" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F39" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="E40" s="33" t="s">
-        <v>60</v>
       </c>
       <c r="F40" s="51"/>
       <c r="J40" s="34" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="51"/>
+      <c r="J42" s="34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="F43" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" s="46" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="F44" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="G44" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="J44" s="46" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="F41" s="51" t="s">
-        <v>214</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="J41" s="46" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>378</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>325</v>
-      </c>
-      <c r="F42" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="G42" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="J42" s="46" t="s">
+    <row r="45" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" s="51"/>
+      <c r="J46" s="34" t="s">
         <v>401</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>326</v>
-      </c>
-      <c r="F43" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="J43" s="20" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="E44" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="51"/>
-      <c r="J44" s="34" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>373</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="51"/>
-      <c r="J45" s="34" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="F46" s="51" t="s">
-        <v>171</v>
-      </c>
-      <c r="G46" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="J46" s="46" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
-      <c r="B47" s="10" t="s">
-        <v>143</v>
+      <c r="B47" s="33" t="s">
+        <v>64</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>318</v>
+        <v>373</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>106</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F47" s="51"/>
       <c r="J47" s="34" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="33" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
-      <c r="B48" s="33" t="s">
-        <v>29</v>
+      <c r="B48" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G48" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="J48" s="34" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="J48" s="46" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="33" t="s">
-        <v>184</v>
+      <c r="B49" s="10" t="s">
+        <v>143</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="F49" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="J49" s="46" t="s">
-        <v>405</v>
+        <v>318</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49" s="51"/>
+      <c r="J49" s="34" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
       <c r="B50" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="G50" s="33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J50" s="34" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="33" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>321</v>
-      </c>
-      <c r="E51" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="F51" s="35" t="s">
-        <v>185</v>
+        <v>278</v>
+      </c>
+      <c r="F51" s="51" t="s">
+        <v>182</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>440</v>
+        <v>404</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
       <c r="B52" s="33" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F52" s="35" t="s">
-        <v>216</v>
+        <v>69</v>
+      </c>
+      <c r="F52" s="51" t="s">
+        <v>215</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="J52" s="46" t="s">
-        <v>441</v>
+        <v>156</v>
+      </c>
+      <c r="J52" s="34" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="33" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>321</v>
       </c>
       <c r="E53" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="J53" s="46" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="28"/>
+      <c r="B54" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="E54" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="J54" s="46" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="28"/>
+      <c r="B55" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="E55" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F55" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="G53" s="33" t="s">
+      <c r="G55" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="J53" s="46" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="10" t="s">
+      <c r="J55" s="46" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
+      <c r="B56" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C54" s="33" t="s">
+      <c r="C56" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="E56" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="F54" s="51"/>
-      <c r="J54" s="34" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="F55" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="G55" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="J55" s="46" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="F56" s="51"/>
       <c r="J56" s="34" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
-      <c r="B57" s="33" t="s">
-        <v>23</v>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F57" s="51"/>
-      <c r="J57" s="34" t="s">
-        <v>446</v>
+        <v>83</v>
+      </c>
+      <c r="F57" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="G57" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="J57" s="46" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="42" t="s">
+        <v>31</v>
+      </c>
       <c r="B58" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58" s="51"/>
       <c r="J58" s="34" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
       <c r="B59" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="33" t="s">
         <v>20</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F59" s="51"/>
       <c r="J59" s="34" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
-      <c r="B60" s="33" t="s">
-        <v>265</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="35" t="s">
+        <v>128</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="F60" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="G60" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="J60" s="46" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="51"/>
+      <c r="J60" s="34" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="33" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="F61" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="G61" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="J61" s="46" t="s">
-        <v>449</v>
+        <v>20</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F61" s="51"/>
+      <c r="J61" s="34" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="B62" s="35" t="s">
-        <v>140</v>
+      <c r="A62" s="28"/>
+      <c r="B62" s="33" t="s">
+        <v>265</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="E62" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="F62" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="G62" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="J62" s="20" t="s">
-        <v>450</v>
+        <v>294</v>
+      </c>
+      <c r="F62" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="G62" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="J62" s="46" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="G63" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="J63" s="46" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="G64" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="28"/>
+      <c r="B65" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C63" s="33" t="s">
+      <c r="C65" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="F63" s="51" t="s">
+      <c r="F65" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="G63" s="33" t="s">
+      <c r="G65" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="J63" s="46" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="28"/>
-      <c r="B64" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="D64" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="F64" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="G64" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="J64" s="46" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F65" s="51"/>
-      <c r="J65" s="34"/>
-    </row>
-    <row r="66" spans="1:10" s="33" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="46" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
       <c r="B66" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F66" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="J66" s="46" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="51"/>
+      <c r="J67" s="34"/>
+    </row>
+    <row r="68" spans="1:10" s="33" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="28"/>
+      <c r="B68" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C68" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="F66" s="51" t="s">
+      <c r="F68" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="G66" s="33" t="s">
+      <c r="G68" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="J66" s="46" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="33" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="28"/>
-      <c r="B67" s="10" t="s">
+      <c r="J68" s="46" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="33" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="28"/>
+      <c r="B69" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C67" s="33" t="s">
+      <c r="C69" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="F67" s="35" t="s">
+      <c r="F69" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="G67" s="49" t="s">
+      <c r="G69" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="J67" s="20" t="s">
+      <c r="J69" s="20" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F70" s="51"/>
+      <c r="J70" s="20" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
-      <c r="B68" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="E68" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="F68" s="51"/>
-      <c r="J68" s="20" t="s">
+    <row r="71" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="F71" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="G71" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="J71" s="20" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="F69" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="G69" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="J69" s="20" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="F70" s="22"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
-      <c r="J70" s="22" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
-      <c r="B71" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="F71" s="22"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="22" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="10" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="D72" s="10"/>
       <c r="E72" s="10" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="F72" s="22"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
       <c r="J72" s="22" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="F73" s="22"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="47" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="F74" s="22"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="22" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="F75" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="G75" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="J75" s="20" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="28"/>
+      <c r="B76" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F76" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="G76" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="J76" s="20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="47" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="28"/>
+      <c r="B77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="35"/>
+      <c r="J77" s="20" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="G78" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="22" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="28"/>
-      <c r="B73" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="C73" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="F73" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="G73" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="J73" s="20" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="33" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
-      <c r="B74" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C74" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="F74" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="G74" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="J74" s="20" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" s="47" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="28"/>
-      <c r="B75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="35"/>
-      <c r="J75" s="20" t="s">
+    <row r="79" spans="1:10" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B79" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="F79" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="G79" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="J79" s="46" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="28"/>
+      <c r="B80" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="F80" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="G80" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="J80" s="46" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E81" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="F81" s="51"/>
+      <c r="J81" s="48" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="45" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="28"/>
+      <c r="B82" s="10"/>
+      <c r="F82" s="51"/>
+      <c r="J82" s="46" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="28"/>
+      <c r="B83" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C83" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F83" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="G83" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="J83" s="46" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
-      <c r="B76" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="F76" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="G76" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="22" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B77" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C77" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="F77" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="G77" s="45" t="s">
-        <v>243</v>
-      </c>
-      <c r="J77" s="46" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="C78" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="F78" s="51" t="s">
-        <v>254</v>
-      </c>
-      <c r="G78" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="J78" s="46" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="E79" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="F79" s="51"/>
-      <c r="J79" s="48" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="45" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
-      <c r="B80" s="10"/>
-      <c r="F80" s="51"/>
-      <c r="J80" s="46" t="s">
+    <row r="84" spans="1:10" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="10"/>
+      <c r="B84" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F84" s="51"/>
+      <c r="J84" s="20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C85" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="F85" s="51"/>
+      <c r="J85" s="59" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
-      <c r="B81" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C81" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="F81" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="G81" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="J81" s="46" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F82" s="51"/>
-      <c r="J82" s="20" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="C83" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="D83" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="F83" s="51"/>
-      <c r="J83" s="57" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="10"/>
-      <c r="C84" s="55"/>
-      <c r="D84" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="F84" s="51"/>
-      <c r="J84" s="57"/>
-    </row>
-    <row r="85" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="10"/>
-      <c r="C85" s="55"/>
-      <c r="D85" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="F85" s="51"/>
-      <c r="J85" s="57"/>
     </row>
     <row r="86" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="10"/>
-      <c r="C86" s="55"/>
+      <c r="C86" s="57"/>
       <c r="D86" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="F86" s="51"/>
+      <c r="J86" s="59"/>
+    </row>
+    <row r="87" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="10"/>
+      <c r="C87" s="57"/>
+      <c r="D87" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F87" s="51"/>
+      <c r="J87" s="59"/>
+    </row>
+    <row r="88" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="10"/>
+      <c r="C88" s="57"/>
+      <c r="D88" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F86" s="51"/>
-      <c r="J86" s="57"/>
-    </row>
-    <row r="87" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="F88" s="51"/>
+      <c r="J88" s="59"/>
+    </row>
+    <row r="89" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="13"/>
-    </row>
-    <row r="88" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="33" t="s">
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="13"/>
+    </row>
+    <row r="90" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="15"/>
+      <c r="B90" s="33" t="s">
         <v>385</v>
       </c>
-      <c r="C88" s="33" t="s">
+      <c r="C90" s="33" t="s">
         <v>295</v>
       </c>
-      <c r="F88" s="51" t="s">
+      <c r="F90" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="G88" s="33" t="s">
+      <c r="G90" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="J88" s="20" t="s">
+      <c r="J90" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="F91" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="G91" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="J91" s="46" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="28" t="s">
-        <v>381</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="C89" s="33" t="s">
-        <v>352</v>
-      </c>
-      <c r="F89" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="G89" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="J89" s="46" t="s">
+    <row r="92" spans="1:10" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="28"/>
+      <c r="B92" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C92" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="F92" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="G92" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="J92" s="46" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C90" s="33" t="s">
-        <v>353</v>
-      </c>
-      <c r="F90" s="35" t="s">
-        <v>236</v>
-      </c>
-      <c r="G90" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="J90" s="46" t="s">
+    <row r="93" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C93" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="F93" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="G93" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="J93" s="46" t="s">
         <v>461</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="33" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="28" t="s">
-        <v>382</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="C91" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="F91" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="G91" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="J91" s="46" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
-      <c r="B92" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="G92" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="H92" s="10"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="22" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
-        <v>383</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="H93" s="10"/>
-      <c r="I93" s="10"/>
-      <c r="J93" s="22" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="94" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="10" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
       <c r="F94" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>247</v>
+        <v>231</v>
+      </c>
+      <c r="G94" s="50" t="s">
+        <v>245</v>
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
-      <c r="J94" s="20" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
+      <c r="J94" s="22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="21" t="s">
+        <v>383</v>
+      </c>
       <c r="B95" s="10" t="s">
-        <v>334</v>
+        <v>250</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
-      <c r="F95" s="52" t="s">
-        <v>236</v>
-      </c>
-      <c r="G95" s="50" t="s">
-        <v>248</v>
+      <c r="F95" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>251</v>
       </c>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
       <c r="J95" s="22" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="36" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+      <c r="B97" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="52" t="s">
+        <v>236</v>
+      </c>
+      <c r="G97" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="22" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="B96" s="37" t="s">
+      <c r="B98" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C96" s="37" t="s">
+      <c r="C98" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="D96" s="37" t="s">
+      <c r="D98" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="F96" s="38"/>
-      <c r="J96" s="38" t="s">
+      <c r="F98" s="38"/>
+      <c r="J98" s="38" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="28"/>
+      <c r="B99" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F99" s="51"/>
+      <c r="J99" s="34" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="28"/>
-      <c r="B97" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C97" s="33" t="s">
-        <v>320</v>
-      </c>
-      <c r="D97" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F97" s="51"/>
-      <c r="J97" s="34" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-      <c r="B98" s="33" t="s">
+    <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15"/>
+      <c r="B100" s="33" t="s">
         <v>351</v>
       </c>
-      <c r="C98" s="33" t="s">
+      <c r="C100" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="D98" s="33" t="s">
+      <c r="D100" s="33" t="s">
         <v>109</v>
-      </c>
-      <c r="F98" s="51"/>
-      <c r="J98" s="20" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="15"/>
-      <c r="B99" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="C99" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="F99" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="G99" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="J99" s="20" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
-      <c r="B100" s="33" t="s">
-        <v>349</v>
-      </c>
-      <c r="C100" s="33" t="s">
-        <v>349</v>
-      </c>
-      <c r="D100" s="33" t="s">
-        <v>110</v>
       </c>
       <c r="F100" s="51"/>
       <c r="J100" s="20" t="s">
-        <v>466</v>
+        <v>418</v>
       </c>
     </row>
     <row r="101" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C101" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="F101" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="G101" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="J101" s="20" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="28"/>
+      <c r="B102" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="C102" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D102" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F102" s="51"/>
+      <c r="J102" s="20" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="15"/>
+      <c r="B103" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C101" s="33" t="s">
+      <c r="C103" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="D101" s="33" t="s">
+      <c r="D103" s="33" t="s">
         <v>111</v>
-      </c>
-      <c r="F101" s="51"/>
-      <c r="J101" s="20" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="28"/>
-      <c r="B102" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="D102" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F102" s="51"/>
-      <c r="J102" s="34" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
-      <c r="B103" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C103" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="D103" s="33" t="s">
-        <v>114</v>
       </c>
       <c r="F103" s="51"/>
       <c r="J103" s="20" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="21" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="28"/>
+      <c r="B104" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F104" s="51"/>
+      <c r="J104" s="34" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="28"/>
+      <c r="B105" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="D105" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F105" s="51"/>
+      <c r="J105" s="20" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B104" s="10" t="s">
+      <c r="B106" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C106" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="D104" s="10" t="s">
+      <c r="D106" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F104" s="22"/>
-      <c r="G104" s="10"/>
-      <c r="H104" s="10"/>
-      <c r="I104" s="10"/>
-      <c r="J104" s="22" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="21"/>
-      <c r="B105" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="22"/>
-      <c r="G105" s="10"/>
-      <c r="H105" s="10"/>
-      <c r="I105" s="10"/>
-      <c r="J105" s="22" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="21"/>
-      <c r="B106" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
       <c r="F106" s="22"/>
       <c r="G106" s="10"/>
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
       <c r="J106" s="22" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="107" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="10" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
@@ -4613,295 +4639,307 @@
       <c r="H107" s="10"/>
       <c r="I107" s="10"/>
       <c r="J107" s="22" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
       <c r="F108" s="22"/>
       <c r="G108" s="10"/>
       <c r="H108" s="10"/>
       <c r="I108" s="10"/>
       <c r="J108" s="22" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="109" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="10" t="s">
-        <v>42</v>
+        <v>372</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
       <c r="F109" s="22"/>
       <c r="G109" s="10"/>
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
       <c r="J109" s="22" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="21"/>
       <c r="B110" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="D110" s="10"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="J110" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="21"/>
+      <c r="B111" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="D111" s="10"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="J111" s="22" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="55" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="21"/>
+      <c r="B112" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="55" t="s">
+        <v>481</v>
+      </c>
+      <c r="F112" s="22"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="J112" s="22" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C110" s="33" t="s">
+      <c r="C113" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="D110" s="33" t="s">
+      <c r="D113" s="33" t="s">
         <v>116</v>
-      </c>
-      <c r="F110" s="51"/>
-      <c r="J110" s="34" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C111" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="D111" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="F111" s="51"/>
-      <c r="J111" s="34" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="E112" s="33" t="s">
-        <v>371</v>
-      </c>
-      <c r="F112" s="51"/>
-      <c r="J112" s="34" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C113" s="33" t="s">
-        <v>343</v>
-      </c>
-      <c r="D113" s="33" t="s">
-        <v>119</v>
       </c>
       <c r="F113" s="51"/>
       <c r="J113" s="34" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B114" s="33" t="s">
-        <v>92</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="C114" s="33" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D114" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F114" s="51"/>
       <c r="J114" s="34" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="28"/>
-      <c r="B115" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C115" s="33" t="s">
-        <v>345</v>
-      </c>
-      <c r="D115" s="33" t="s">
-        <v>122</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>371</v>
       </c>
       <c r="F115" s="51"/>
       <c r="J115" s="34" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C116" s="33" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D116" s="33" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F116" s="51"/>
-      <c r="J116" s="34"/>
-    </row>
-    <row r="117" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="15"/>
+      <c r="J116" s="34" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B117" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C117" s="33" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D117" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F117" s="51"/>
       <c r="J117" s="34" t="s">
-        <v>474</v>
+        <v>411</v>
       </c>
     </row>
     <row r="118" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="28"/>
       <c r="B118" s="33" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="C118" s="33" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D118" s="33" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F118" s="51"/>
       <c r="J118" s="34" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="119" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
+      <c r="A119" s="15"/>
       <c r="B119" s="33" t="s">
-        <v>268</v>
+        <v>89</v>
       </c>
       <c r="C119" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D119" s="33" t="s">
-        <v>269</v>
+        <v>125</v>
       </c>
       <c r="F119" s="51"/>
-      <c r="J119" s="34" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="F120" s="13"/>
-      <c r="J120" s="13"/>
-    </row>
-    <row r="121" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J119" s="34"/>
+    </row>
+    <row r="120" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="15"/>
+      <c r="B120" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C120" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="D120" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F120" s="51"/>
+      <c r="J120" s="34" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="28"/>
       <c r="B121" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C121" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="D121" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F121" s="51"/>
+      <c r="J121" s="34" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="28"/>
+      <c r="B122" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="C122" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="D122" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="F122" s="51"/>
+      <c r="J122" s="34" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="F123" s="13"/>
+      <c r="J123" s="13"/>
+    </row>
+    <row r="124" spans="1:10" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="28"/>
+      <c r="B124" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="C121" s="33" t="s">
+      <c r="C124" s="33" t="s">
         <v>317</v>
       </c>
-      <c r="F121" s="35" t="s">
+      <c r="F124" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="G121" s="33" t="s">
+      <c r="G124" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="J121" s="46" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="28"/>
-      <c r="B122" s="32" t="s">
+      <c r="J124" s="46" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="28"/>
+      <c r="B125" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C122" s="33" t="s">
+      <c r="C125" s="33" t="s">
         <v>317</v>
       </c>
-      <c r="F122" s="35" t="s">
-        <v>477</v>
-      </c>
-      <c r="G122" s="33" t="s">
+      <c r="F125" s="35" t="s">
+        <v>476</v>
+      </c>
+      <c r="G125" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="J122" s="51" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="11" t="s">
+      <c r="J125" s="51" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-      <c r="G123" s="12"/>
-      <c r="H123" s="12"/>
-      <c r="I123" s="12"/>
-      <c r="J123" s="43"/>
-    </row>
-    <row r="124" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
-      <c r="F124" s="10"/>
-      <c r="G124" s="10"/>
-      <c r="H124" s="10"/>
-      <c r="I124" s="10"/>
-      <c r="J124" s="44"/>
-    </row>
-    <row r="125" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10"/>
-      <c r="F125" s="10"/>
-      <c r="G125" s="10"/>
-      <c r="H125" s="10"/>
-      <c r="I125" s="10"/>
-      <c r="J125" s="44"/>
-    </row>
-    <row r="126" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="10"/>
-      <c r="F126" s="10"/>
-      <c r="G126" s="10"/>
-      <c r="H126" s="10"/>
-      <c r="I126" s="10"/>
-      <c r="J126" s="44"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+      <c r="I126" s="12"/>
+      <c r="J126" s="43"/>
     </row>
     <row r="127" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -4914,7 +4952,9 @@
       <c r="J127" s="44"/>
     </row>
     <row r="128" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="21"/>
+      <c r="A128" s="22" t="s">
+        <v>135</v>
+      </c>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
       <c r="D128" s="10"/>
@@ -4923,80 +4963,84 @@
       <c r="G128" s="10"/>
       <c r="H128" s="10"/>
       <c r="I128" s="10"/>
-      <c r="J128" s="20"/>
+      <c r="J128" s="44"/>
     </row>
     <row r="129" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="55" t="s">
+      <c r="A129" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="44"/>
+    </row>
+    <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130" s="10"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="J130" s="44"/>
+    </row>
+    <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="20"/>
+    </row>
+    <row r="132" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="B129" s="55"/>
-      <c r="C129" s="55"/>
-      <c r="J129" s="34"/>
-    </row>
-    <row r="130" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="55"/>
-      <c r="B130" s="55"/>
-      <c r="C130" s="55"/>
-      <c r="J130" s="34"/>
-    </row>
-    <row r="131" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="55"/>
-      <c r="B131" s="55"/>
-      <c r="C131" s="55"/>
-      <c r="J131" s="34"/>
-    </row>
-    <row r="132" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="55"/>
-      <c r="B132" s="55"/>
-      <c r="C132" s="55"/>
+      <c r="B132" s="57"/>
+      <c r="C132" s="57"/>
       <c r="J132" s="34"/>
     </row>
     <row r="133" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="55"/>
-      <c r="B133" s="55"/>
-      <c r="C133" s="55"/>
+      <c r="A133" s="57"/>
+      <c r="B133" s="57"/>
+      <c r="C133" s="57"/>
       <c r="J133" s="34"/>
     </row>
-    <row r="134" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="55"/>
-      <c r="B134" s="55"/>
-      <c r="C134" s="55"/>
-      <c r="D134" s="33"/>
-      <c r="E134" s="33"/>
-      <c r="F134" s="33"/>
-      <c r="G134" s="33"/>
-      <c r="H134" s="33"/>
-      <c r="I134" s="33"/>
+    <row r="134" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="57"/>
+      <c r="B134" s="57"/>
+      <c r="C134" s="57"/>
       <c r="J134" s="34"/>
     </row>
-    <row r="135" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="33"/>
-      <c r="B135" s="33"/>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
-      <c r="E135" s="33"/>
-      <c r="F135" s="33"/>
-      <c r="G135" s="33"/>
-      <c r="H135" s="33"/>
-      <c r="I135" s="33"/>
+    <row r="135" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="57"/>
+      <c r="B135" s="57"/>
+      <c r="C135" s="57"/>
       <c r="J135" s="34"/>
     </row>
-    <row r="136" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="33"/>
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
-      <c r="E136" s="33"/>
-      <c r="F136" s="33"/>
-      <c r="G136" s="33"/>
-      <c r="H136" s="33"/>
-      <c r="I136" s="33"/>
+    <row r="136" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="57"/>
+      <c r="B136" s="57"/>
+      <c r="C136" s="57"/>
       <c r="J136" s="34"/>
     </row>
     <row r="137" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="33"/>
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
+      <c r="A137" s="57"/>
+      <c r="B137" s="57"/>
+      <c r="C137" s="57"/>
       <c r="D137" s="33"/>
       <c r="E137" s="33"/>
       <c r="F137" s="33"/>
@@ -5009,6 +5053,7 @@
       <c r="A138" s="33"/>
       <c r="B138" s="33"/>
       <c r="C138" s="33"/>
+      <c r="D138" s="33"/>
       <c r="E138" s="33"/>
       <c r="F138" s="33"/>
       <c r="G138" s="33"/>
@@ -5026,34 +5071,42 @@
       <c r="G139" s="33"/>
       <c r="H139" s="33"/>
       <c r="I139" s="33"/>
-      <c r="J139" s="28"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="3"/>
-      <c r="B140" s="4"/>
-      <c r="C140" s="30"/>
-      <c r="D140" s="16"/>
-      <c r="E140" s="4"/>
-      <c r="H140" s="24"/>
-      <c r="I140" s="24"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" s="3"/>
-      <c r="B141" s="4"/>
-      <c r="C141" s="30"/>
-      <c r="D141" s="16"/>
-      <c r="E141" s="4"/>
-      <c r="H141" s="24"/>
-      <c r="I141" s="24"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" s="3"/>
-      <c r="B142" s="4"/>
-      <c r="C142" s="30"/>
-      <c r="D142" s="16"/>
-      <c r="E142" s="4"/>
-      <c r="H142" s="24"/>
-      <c r="I142" s="24"/>
+      <c r="J139" s="34"/>
+    </row>
+    <row r="140" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="33"/>
+      <c r="B140" s="33"/>
+      <c r="C140" s="33"/>
+      <c r="D140" s="33"/>
+      <c r="E140" s="33"/>
+      <c r="F140" s="33"/>
+      <c r="G140" s="33"/>
+      <c r="H140" s="33"/>
+      <c r="I140" s="33"/>
+      <c r="J140" s="34"/>
+    </row>
+    <row r="141" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="33"/>
+      <c r="B141" s="33"/>
+      <c r="C141" s="33"/>
+      <c r="E141" s="33"/>
+      <c r="F141" s="33"/>
+      <c r="G141" s="33"/>
+      <c r="H141" s="33"/>
+      <c r="I141" s="33"/>
+      <c r="J141" s="34"/>
+    </row>
+    <row r="142" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="33"/>
+      <c r="B142" s="33"/>
+      <c r="C142" s="33"/>
+      <c r="D142" s="33"/>
+      <c r="E142" s="33"/>
+      <c r="F142" s="33"/>
+      <c r="G142" s="33"/>
+      <c r="H142" s="33"/>
+      <c r="I142" s="33"/>
+      <c r="J142" s="28"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
@@ -5131,7 +5184,7 @@
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="30"/>
-      <c r="D151" s="19"/>
+      <c r="D151" s="16"/>
       <c r="E151" s="4"/>
       <c r="H151" s="24"/>
       <c r="I151" s="24"/>
@@ -5158,7 +5211,7 @@
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="30"/>
-      <c r="D154" s="16"/>
+      <c r="D154" s="19"/>
       <c r="E154" s="4"/>
       <c r="H154" s="24"/>
       <c r="I154" s="24"/>
@@ -5568,27 +5621,54 @@
       <c r="H199" s="24"/>
       <c r="I199" s="24"/>
     </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="3"/>
+      <c r="B200" s="4"/>
+      <c r="C200" s="30"/>
+      <c r="D200" s="16"/>
+      <c r="E200" s="4"/>
+      <c r="H200" s="24"/>
+      <c r="I200" s="24"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="3"/>
+      <c r="B201" s="4"/>
+      <c r="C201" s="30"/>
+      <c r="D201" s="16"/>
+      <c r="E201" s="4"/>
+      <c r="H201" s="24"/>
+      <c r="I201" s="24"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" s="3"/>
+      <c r="B202" s="4"/>
+      <c r="C202" s="30"/>
+      <c r="D202" s="16"/>
+      <c r="E202" s="4"/>
+      <c r="H202" s="24"/>
+      <c r="I202" s="24"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A129:C134"/>
+    <mergeCell ref="A132:C137"/>
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="J83:J86"/>
-    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="J85:J88"/>
+    <mergeCell ref="C85:C88"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G69" r:id="rId1"/>
-    <hyperlink ref="G78" r:id="rId2"/>
-    <hyperlink ref="G92" r:id="rId3"/>
-    <hyperlink ref="G91" r:id="rId4"/>
-    <hyperlink ref="G67" r:id="rId5"/>
-    <hyperlink ref="G60" r:id="rId6"/>
-    <hyperlink ref="G76" r:id="rId7"/>
-    <hyperlink ref="G95" r:id="rId8"/>
+    <hyperlink ref="G71" r:id="rId1"/>
+    <hyperlink ref="G80" r:id="rId2"/>
+    <hyperlink ref="G94" r:id="rId3"/>
+    <hyperlink ref="G93" r:id="rId4"/>
+    <hyperlink ref="G69" r:id="rId5"/>
+    <hyperlink ref="G62" r:id="rId6"/>
+    <hyperlink ref="G78" r:id="rId7"/>
+    <hyperlink ref="G97" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>

</xml_diff>